<commit_message>
0.0.4: fix error on List of primitive to json.
</commit_message>
<xml_diff>
--- a/meta/api/GetTableSample2.xlsx
+++ b/meta/api/GetTableSample2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E266A33-1CDA-7A47-B43B-E5830795550D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A223CE-05A1-9944-B228-775FD33AD02C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="1040" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14540" yWindow="460" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -28,11 +28,11 @@
     <definedName name="isNullable">config!$F$5:$F$6</definedName>
     <definedName name="others">config!$G$5:$G$6</definedName>
     <definedName name="Submit有無">config!$B$5:$B$6</definedName>
-    <definedName name="threeAlters">[2]config!$H$5:$H$7</definedName>
+    <definedName name="threeAlters">[1]config!$H$5:$H$7</definedName>
     <definedName name="Validate実装パターン">config!$A$5:$A$6</definedName>
     <definedName name="チェック種別">config!$D$5:$D$49</definedName>
     <definedName name="型">config!#REF!</definedName>
-    <definedName name="形式タイプ">[1]telegramConfig!$D$6:$D$27</definedName>
+    <definedName name="形式タイプ">[2]telegramConfig!$D$6:$D$27</definedName>
     <definedName name="項目型" localSheetId="1">config!#REF!</definedName>
     <definedName name="項目型" localSheetId="2">config!#REF!</definedName>
     <definedName name="項目型">config!#REF!</definedName>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="201">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2257,6 +2257,32 @@
   </si>
   <si>
     <t>listOf&lt;CodeDefinition&gt;()</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Long</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>myLong</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Long値</t>
+    <rPh sb="4" eb="5">
+      <t xml:space="preserve">チ </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>myArray</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Longの配列</t>
+    <rPh sb="5" eb="7">
+      <t xml:space="preserve">ハイレツ </t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3479,6 +3505,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="59" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3683,9 +3712,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="59" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3777,6 +3803,38 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="process"/>
+      <sheetName val="post_input"/>
+      <sheetName val="post_output"/>
+      <sheetName val="readme"/>
+      <sheetName val="config"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="5">
+          <cell r="H5" t="str">
+            <v>YES</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="H6" t="str">
+            <v>NOT</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3898,38 +3956,6 @@
         <row r="27">
           <cell r="D27" t="str">
             <v>月日 (MM/dd)</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="process"/>
-      <sheetName val="post_input"/>
-      <sheetName val="post_output"/>
-      <sheetName val="readme"/>
-      <sheetName val="config"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
-        <row r="5">
-          <cell r="H5" t="str">
-            <v>YES</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="H6" t="str">
-            <v>NOT</v>
           </cell>
         </row>
       </sheetData>
@@ -4309,137 +4335,137 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="137" t="s">
+      <c r="A5" s="138" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="137"/>
-      <c r="C5" s="137"/>
-      <c r="D5" s="137"/>
-      <c r="E5" s="137"/>
+      <c r="B5" s="138"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="138"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="95"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="141" t="s">
+      <c r="A6" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="142"/>
-      <c r="C6" s="143"/>
-      <c r="D6" s="138" t="s">
+      <c r="B6" s="143"/>
+      <c r="C6" s="144"/>
+      <c r="D6" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="E6" s="138"/>
+      <c r="E6" s="139"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="137" t="s">
+      <c r="A7" s="138" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="137"/>
-      <c r="C7" s="137"/>
-      <c r="D7" s="138" t="s">
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="139" t="s">
         <v>133</v>
       </c>
-      <c r="E7" s="138"/>
+      <c r="E7" s="139"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="137" t="s">
+      <c r="A8" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="137"/>
-      <c r="C8" s="137"/>
-      <c r="D8" s="138" t="s">
+      <c r="B8" s="138"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="E8" s="138"/>
+      <c r="E8" s="139"/>
       <c r="F8" s="95"/>
       <c r="G8" s="95"/>
       <c r="H8" s="95"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="137" t="s">
+      <c r="A9" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="137"/>
-      <c r="C9" s="137"/>
-      <c r="D9" s="138" t="s">
+      <c r="B9" s="138"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="139" t="s">
         <v>180</v>
       </c>
-      <c r="E9" s="138"/>
+      <c r="E9" s="139"/>
       <c r="F9" s="95"/>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="137" t="s">
+      <c r="A10" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="137"/>
-      <c r="C10" s="137"/>
-      <c r="D10" s="138"/>
-      <c r="E10" s="138"/>
+      <c r="B10" s="138"/>
+      <c r="C10" s="138"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="139"/>
       <c r="F10" s="95"/>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="137" t="s">
+      <c r="A11" s="138" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="137"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="138" t="s">
+      <c r="B11" s="138"/>
+      <c r="C11" s="138"/>
+      <c r="D11" s="139" t="s">
         <v>179</v>
       </c>
-      <c r="E11" s="138"/>
+      <c r="E11" s="139"/>
       <c r="F11" s="95"/>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="144" t="s">
+      <c r="A12" s="145" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="144"/>
-      <c r="C12" s="144"/>
-      <c r="D12" s="139" t="s">
+      <c r="B12" s="145"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="E12" s="139"/>
+      <c r="E12" s="140"/>
       <c r="F12" s="95" t="s">
         <v>137</v>
       </c>
       <c r="G12" s="54"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="144" t="s">
+      <c r="A13" s="145" t="s">
         <v>167</v>
       </c>
-      <c r="B13" s="144"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="139" t="s">
+      <c r="B13" s="145"/>
+      <c r="C13" s="145"/>
+      <c r="D13" s="140" t="s">
         <v>165</v>
       </c>
-      <c r="E13" s="139"/>
+      <c r="E13" s="140"/>
       <c r="F13" s="95" t="s">
         <v>166</v>
       </c>
       <c r="G13" s="54"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="144" t="s">
+      <c r="A14" s="145" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="144"/>
-      <c r="C14" s="144"/>
-      <c r="D14" s="140"/>
-      <c r="E14" s="139"/>
+      <c r="B14" s="145"/>
+      <c r="C14" s="145"/>
+      <c r="D14" s="141"/>
+      <c r="E14" s="140"/>
       <c r="F14" s="54" t="s">
         <v>156</v>
       </c>
@@ -4447,15 +4473,15 @@
       <c r="H14" s="95"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="144" t="s">
+      <c r="A15" s="145" t="s">
         <v>171</v>
       </c>
-      <c r="B15" s="144"/>
-      <c r="C15" s="144"/>
-      <c r="D15" s="140" t="s">
+      <c r="B15" s="145"/>
+      <c r="C15" s="145"/>
+      <c r="D15" s="141" t="s">
         <v>181</v>
       </c>
-      <c r="E15" s="139"/>
+      <c r="E15" s="140"/>
       <c r="F15" s="54" t="s">
         <v>173</v>
       </c>
@@ -4463,13 +4489,13 @@
       <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="145" t="s">
         <v>170</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="140"/>
-      <c r="E16" s="139"/>
+      <c r="B16" s="145"/>
+      <c r="C16" s="145"/>
+      <c r="D16" s="141"/>
+      <c r="E16" s="140"/>
       <c r="F16" s="54" t="s">
         <v>172</v>
       </c>
@@ -4477,15 +4503,15 @@
       <c r="H16" s="95"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="144" t="s">
+      <c r="A17" s="145" t="s">
         <v>169</v>
       </c>
-      <c r="B17" s="144"/>
-      <c r="C17" s="144"/>
-      <c r="D17" s="140" t="s">
+      <c r="B17" s="145"/>
+      <c r="C17" s="145"/>
+      <c r="D17" s="141" t="s">
         <v>174</v>
       </c>
-      <c r="E17" s="139"/>
+      <c r="E17" s="140"/>
       <c r="F17" s="54" t="s">
         <v>168</v>
       </c>
@@ -4493,19 +4519,19 @@
       <c r="H17" s="95"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="181" t="s">
+      <c r="A18" s="182" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="182"/>
-      <c r="C18" s="183"/>
+      <c r="B18" s="183"/>
+      <c r="C18" s="184"/>
       <c r="D18" s="114"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="167" t="s">
+      <c r="A19" s="168" t="s">
         <v>139</v>
       </c>
-      <c r="B19" s="168"/>
-      <c r="C19" s="169"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="170"/>
       <c r="D19" s="100"/>
       <c r="E19" t="s">
         <v>140</v>
@@ -4523,15 +4549,15 @@
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="178" t="s">
+      <c r="A21" s="179" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="179"/>
-      <c r="C21" s="179"/>
-      <c r="D21" s="179"/>
-      <c r="E21" s="179"/>
-      <c r="F21" s="179"/>
-      <c r="G21" s="180"/>
+      <c r="B21" s="180"/>
+      <c r="C21" s="180"/>
+      <c r="D21" s="180"/>
+      <c r="E21" s="180"/>
+      <c r="F21" s="180"/>
+      <c r="G21" s="181"/>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="101" t="s">
@@ -4579,28 +4605,28 @@
       <c r="C25"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="177" t="s">
+      <c r="A26" s="178" t="s">
         <v>148</v>
       </c>
-      <c r="B26" s="177"/>
-      <c r="C26" s="177"/>
-      <c r="D26" s="177"/>
-      <c r="E26" s="177"/>
-      <c r="F26" s="177"/>
-      <c r="G26" s="177"/>
+      <c r="B26" s="178"/>
+      <c r="C26" s="178"/>
+      <c r="D26" s="178"/>
+      <c r="E26" s="178"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="178"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="171" t="s">
+      <c r="B27" s="172" t="s">
         <v>143</v>
       </c>
-      <c r="C27" s="172"/>
-      <c r="D27" s="172"/>
-      <c r="E27" s="172"/>
-      <c r="F27" s="172"/>
-      <c r="G27" s="173"/>
+      <c r="C27" s="173"/>
+      <c r="D27" s="173"/>
+      <c r="E27" s="173"/>
+      <c r="F27" s="173"/>
+      <c r="G27" s="174"/>
       <c r="H27" s="105"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -4611,12 +4637,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="116"/>
-      <c r="B28" s="160"/>
-      <c r="C28" s="160"/>
-      <c r="D28" s="160"/>
-      <c r="E28" s="160"/>
-      <c r="F28" s="160"/>
-      <c r="G28" s="160"/>
+      <c r="B28" s="161"/>
+      <c r="C28" s="161"/>
+      <c r="D28" s="161"/>
+      <c r="E28" s="161"/>
+      <c r="F28" s="161"/>
+      <c r="G28" s="161"/>
       <c r="H28" s="112"/>
       <c r="I28" s="112"/>
       <c r="J28" s="112"/>
@@ -4627,12 +4653,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="117"/>
-      <c r="B29" s="156"/>
-      <c r="C29" s="156"/>
-      <c r="D29" s="156"/>
-      <c r="E29" s="156"/>
-      <c r="F29" s="156"/>
-      <c r="G29" s="156"/>
+      <c r="B29" s="157"/>
+      <c r="C29" s="157"/>
+      <c r="D29" s="157"/>
+      <c r="E29" s="157"/>
+      <c r="F29" s="157"/>
+      <c r="G29" s="157"/>
       <c r="H29" s="112"/>
       <c r="I29" s="112"/>
       <c r="J29" s="112"/>
@@ -4643,12 +4669,12 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="118"/>
-      <c r="B30" s="158"/>
-      <c r="C30" s="158"/>
-      <c r="D30" s="158"/>
-      <c r="E30" s="158"/>
-      <c r="F30" s="158"/>
-      <c r="G30" s="158"/>
+      <c r="B30" s="159"/>
+      <c r="C30" s="159"/>
+      <c r="D30" s="159"/>
+      <c r="E30" s="159"/>
+      <c r="F30" s="159"/>
+      <c r="G30" s="159"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -4661,28 +4687,28 @@
       <c r="C31"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="174" t="s">
+      <c r="A32" s="175" t="s">
         <v>149</v>
       </c>
-      <c r="B32" s="175"/>
-      <c r="C32" s="175"/>
-      <c r="D32" s="175"/>
-      <c r="E32" s="175"/>
-      <c r="F32" s="175"/>
-      <c r="G32" s="176"/>
+      <c r="B32" s="176"/>
+      <c r="C32" s="176"/>
+      <c r="D32" s="176"/>
+      <c r="E32" s="176"/>
+      <c r="F32" s="176"/>
+      <c r="G32" s="177"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="151" t="s">
+      <c r="B33" s="152" t="s">
         <v>144</v>
       </c>
-      <c r="C33" s="151"/>
-      <c r="D33" s="151"/>
-      <c r="E33" s="151"/>
-      <c r="F33" s="151"/>
-      <c r="G33" s="151"/>
+      <c r="C33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="152"/>
       <c r="H33" s="105"/>
       <c r="I33" s="105"/>
       <c r="J33" s="105"/>
@@ -4693,12 +4719,12 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="116"/>
-      <c r="B34" s="152"/>
-      <c r="C34" s="152"/>
-      <c r="D34" s="152"/>
-      <c r="E34" s="152"/>
-      <c r="F34" s="152"/>
-      <c r="G34" s="152"/>
+      <c r="B34" s="153"/>
+      <c r="C34" s="153"/>
+      <c r="D34" s="153"/>
+      <c r="E34" s="153"/>
+      <c r="F34" s="153"/>
+      <c r="G34" s="153"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -4709,12 +4735,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="117"/>
-      <c r="B35" s="153"/>
-      <c r="C35" s="153"/>
-      <c r="D35" s="153"/>
-      <c r="E35" s="153"/>
-      <c r="F35" s="153"/>
-      <c r="G35" s="153"/>
+      <c r="B35" s="154"/>
+      <c r="C35" s="154"/>
+      <c r="D35" s="154"/>
+      <c r="E35" s="154"/>
+      <c r="F35" s="154"/>
+      <c r="G35" s="154"/>
       <c r="H35" s="112"/>
       <c r="I35" s="112"/>
       <c r="J35" s="112"/>
@@ -4725,12 +4751,12 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="118"/>
-      <c r="B36" s="154"/>
-      <c r="C36" s="154"/>
-      <c r="D36" s="154"/>
-      <c r="E36" s="154"/>
-      <c r="F36" s="154"/>
-      <c r="G36" s="154"/>
+      <c r="B36" s="155"/>
+      <c r="C36" s="155"/>
+      <c r="D36" s="155"/>
+      <c r="E36" s="155"/>
+      <c r="F36" s="155"/>
+      <c r="G36" s="155"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -4755,28 +4781,28 @@
       <c r="M37"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="174" t="s">
+      <c r="A38" s="175" t="s">
         <v>150</v>
       </c>
-      <c r="B38" s="175"/>
-      <c r="C38" s="175"/>
-      <c r="D38" s="175"/>
-      <c r="E38" s="175"/>
-      <c r="F38" s="175"/>
-      <c r="G38" s="176"/>
+      <c r="B38" s="176"/>
+      <c r="C38" s="176"/>
+      <c r="D38" s="176"/>
+      <c r="E38" s="176"/>
+      <c r="F38" s="176"/>
+      <c r="G38" s="177"/>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="151" t="s">
+      <c r="B39" s="152" t="s">
         <v>145</v>
       </c>
-      <c r="C39" s="151"/>
-      <c r="D39" s="151"/>
-      <c r="E39" s="151"/>
-      <c r="F39" s="151"/>
-      <c r="G39" s="151"/>
+      <c r="C39" s="152"/>
+      <c r="D39" s="152"/>
+      <c r="E39" s="152"/>
+      <c r="F39" s="152"/>
+      <c r="G39" s="152"/>
       <c r="H39" s="105"/>
       <c r="I39" s="105"/>
       <c r="J39" s="105"/>
@@ -4787,12 +4813,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="116"/>
-      <c r="B40" s="152"/>
-      <c r="C40" s="152"/>
-      <c r="D40" s="152"/>
-      <c r="E40" s="152"/>
-      <c r="F40" s="152"/>
-      <c r="G40" s="155"/>
+      <c r="B40" s="153"/>
+      <c r="C40" s="153"/>
+      <c r="D40" s="153"/>
+      <c r="E40" s="153"/>
+      <c r="F40" s="153"/>
+      <c r="G40" s="156"/>
       <c r="H40" s="112"/>
       <c r="I40" s="112"/>
       <c r="J40" s="112"/>
@@ -4803,12 +4829,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="117"/>
-      <c r="B41" s="156"/>
-      <c r="C41" s="156"/>
-      <c r="D41" s="156"/>
-      <c r="E41" s="156"/>
-      <c r="F41" s="156"/>
-      <c r="G41" s="157"/>
+      <c r="B41" s="157"/>
+      <c r="C41" s="157"/>
+      <c r="D41" s="157"/>
+      <c r="E41" s="157"/>
+      <c r="F41" s="157"/>
+      <c r="G41" s="158"/>
       <c r="H41" s="112"/>
       <c r="I41" s="112"/>
       <c r="J41" s="112"/>
@@ -4819,12 +4845,12 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="118"/>
-      <c r="B42" s="158"/>
-      <c r="C42" s="158"/>
-      <c r="D42" s="158"/>
-      <c r="E42" s="158"/>
-      <c r="F42" s="158"/>
-      <c r="G42" s="159"/>
+      <c r="B42" s="159"/>
+      <c r="C42" s="159"/>
+      <c r="D42" s="159"/>
+      <c r="E42" s="159"/>
+      <c r="F42" s="159"/>
+      <c r="G42" s="160"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -4859,217 +4885,217 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="164" t="s">
+      <c r="A45" s="165" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="170"/>
-      <c r="C45" s="164" t="s">
+      <c r="B45" s="171"/>
+      <c r="C45" s="165" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="165"/>
-      <c r="E45" s="166"/>
+      <c r="D45" s="166"/>
+      <c r="E45" s="167"/>
       <c r="F45" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="161"/>
-      <c r="B46" s="163"/>
-      <c r="C46" s="161"/>
-      <c r="D46" s="162"/>
-      <c r="E46" s="163"/>
+      <c r="A46" s="162"/>
+      <c r="B46" s="164"/>
+      <c r="C46" s="162"/>
+      <c r="D46" s="163"/>
+      <c r="E46" s="164"/>
       <c r="F46" s="49"/>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="145"/>
-      <c r="B47" s="147"/>
-      <c r="C47" s="145"/>
-      <c r="D47" s="146"/>
-      <c r="E47" s="147"/>
+      <c r="A47" s="146"/>
+      <c r="B47" s="148"/>
+      <c r="C47" s="146"/>
+      <c r="D47" s="147"/>
+      <c r="E47" s="148"/>
       <c r="F47" s="49"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="145"/>
-      <c r="B48" s="147"/>
-      <c r="C48" s="145"/>
-      <c r="D48" s="146"/>
-      <c r="E48" s="147"/>
+      <c r="A48" s="146"/>
+      <c r="B48" s="148"/>
+      <c r="C48" s="146"/>
+      <c r="D48" s="147"/>
+      <c r="E48" s="148"/>
       <c r="F48" s="49"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="145"/>
-      <c r="B49" s="147"/>
-      <c r="C49" s="145"/>
-      <c r="D49" s="146"/>
-      <c r="E49" s="147"/>
+      <c r="A49" s="146"/>
+      <c r="B49" s="148"/>
+      <c r="C49" s="146"/>
+      <c r="D49" s="147"/>
+      <c r="E49" s="148"/>
       <c r="F49" s="49"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="145"/>
-      <c r="B50" s="147"/>
-      <c r="C50" s="145"/>
-      <c r="D50" s="146"/>
-      <c r="E50" s="147"/>
+      <c r="A50" s="146"/>
+      <c r="B50" s="148"/>
+      <c r="C50" s="146"/>
+      <c r="D50" s="147"/>
+      <c r="E50" s="148"/>
       <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="145"/>
-      <c r="B51" s="147"/>
-      <c r="C51" s="145"/>
-      <c r="D51" s="146"/>
-      <c r="E51" s="147"/>
+      <c r="A51" s="146"/>
+      <c r="B51" s="148"/>
+      <c r="C51" s="146"/>
+      <c r="D51" s="147"/>
+      <c r="E51" s="148"/>
       <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="145"/>
-      <c r="B52" s="147"/>
-      <c r="C52" s="145"/>
-      <c r="D52" s="146"/>
-      <c r="E52" s="147"/>
+      <c r="A52" s="146"/>
+      <c r="B52" s="148"/>
+      <c r="C52" s="146"/>
+      <c r="D52" s="147"/>
+      <c r="E52" s="148"/>
       <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="145"/>
-      <c r="B53" s="147"/>
-      <c r="C53" s="145"/>
-      <c r="D53" s="146"/>
-      <c r="E53" s="147"/>
+      <c r="A53" s="146"/>
+      <c r="B53" s="148"/>
+      <c r="C53" s="146"/>
+      <c r="D53" s="147"/>
+      <c r="E53" s="148"/>
       <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="145"/>
-      <c r="B54" s="147"/>
-      <c r="C54" s="145"/>
-      <c r="D54" s="146"/>
-      <c r="E54" s="147"/>
+      <c r="A54" s="146"/>
+      <c r="B54" s="148"/>
+      <c r="C54" s="146"/>
+      <c r="D54" s="147"/>
+      <c r="E54" s="148"/>
       <c r="F54" s="49"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="145"/>
-      <c r="B55" s="147"/>
-      <c r="C55" s="145"/>
-      <c r="D55" s="146"/>
-      <c r="E55" s="147"/>
+      <c r="A55" s="146"/>
+      <c r="B55" s="148"/>
+      <c r="C55" s="146"/>
+      <c r="D55" s="147"/>
+      <c r="E55" s="148"/>
       <c r="F55" s="49"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="145"/>
-      <c r="B56" s="147"/>
-      <c r="C56" s="145"/>
-      <c r="D56" s="146"/>
-      <c r="E56" s="147"/>
+      <c r="A56" s="146"/>
+      <c r="B56" s="148"/>
+      <c r="C56" s="146"/>
+      <c r="D56" s="147"/>
+      <c r="E56" s="148"/>
       <c r="F56" s="49"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="145"/>
-      <c r="B57" s="147"/>
-      <c r="C57" s="145"/>
-      <c r="D57" s="146"/>
-      <c r="E57" s="147"/>
+      <c r="A57" s="146"/>
+      <c r="B57" s="148"/>
+      <c r="C57" s="146"/>
+      <c r="D57" s="147"/>
+      <c r="E57" s="148"/>
       <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="145"/>
-      <c r="B58" s="147"/>
-      <c r="C58" s="145"/>
-      <c r="D58" s="146"/>
-      <c r="E58" s="147"/>
+      <c r="A58" s="146"/>
+      <c r="B58" s="148"/>
+      <c r="C58" s="146"/>
+      <c r="D58" s="147"/>
+      <c r="E58" s="148"/>
       <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="145"/>
-      <c r="B59" s="147"/>
-      <c r="C59" s="145"/>
-      <c r="D59" s="146"/>
-      <c r="E59" s="147"/>
+      <c r="A59" s="146"/>
+      <c r="B59" s="148"/>
+      <c r="C59" s="146"/>
+      <c r="D59" s="147"/>
+      <c r="E59" s="148"/>
       <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="145"/>
-      <c r="B60" s="147"/>
-      <c r="C60" s="145"/>
-      <c r="D60" s="146"/>
-      <c r="E60" s="147"/>
+      <c r="A60" s="146"/>
+      <c r="B60" s="148"/>
+      <c r="C60" s="146"/>
+      <c r="D60" s="147"/>
+      <c r="E60" s="148"/>
       <c r="F60" s="49"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="145"/>
-      <c r="B61" s="147"/>
-      <c r="C61" s="145"/>
-      <c r="D61" s="146"/>
-      <c r="E61" s="147"/>
+      <c r="A61" s="146"/>
+      <c r="B61" s="148"/>
+      <c r="C61" s="146"/>
+      <c r="D61" s="147"/>
+      <c r="E61" s="148"/>
       <c r="F61" s="49"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="145"/>
-      <c r="B62" s="147"/>
-      <c r="C62" s="145"/>
-      <c r="D62" s="146"/>
-      <c r="E62" s="147"/>
+      <c r="A62" s="146"/>
+      <c r="B62" s="148"/>
+      <c r="C62" s="146"/>
+      <c r="D62" s="147"/>
+      <c r="E62" s="148"/>
       <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="145"/>
-      <c r="B63" s="147"/>
-      <c r="C63" s="145"/>
-      <c r="D63" s="146"/>
-      <c r="E63" s="147"/>
+      <c r="A63" s="146"/>
+      <c r="B63" s="148"/>
+      <c r="C63" s="146"/>
+      <c r="D63" s="147"/>
+      <c r="E63" s="148"/>
       <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="145"/>
-      <c r="B64" s="147"/>
-      <c r="C64" s="145"/>
-      <c r="D64" s="146"/>
-      <c r="E64" s="147"/>
+      <c r="A64" s="146"/>
+      <c r="B64" s="148"/>
+      <c r="C64" s="146"/>
+      <c r="D64" s="147"/>
+      <c r="E64" s="148"/>
       <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="145"/>
-      <c r="B65" s="147"/>
-      <c r="C65" s="145"/>
-      <c r="D65" s="146"/>
-      <c r="E65" s="147"/>
+      <c r="A65" s="146"/>
+      <c r="B65" s="148"/>
+      <c r="C65" s="146"/>
+      <c r="D65" s="147"/>
+      <c r="E65" s="148"/>
       <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="145"/>
-      <c r="B66" s="147"/>
-      <c r="C66" s="145"/>
-      <c r="D66" s="146"/>
-      <c r="E66" s="147"/>
+      <c r="A66" s="146"/>
+      <c r="B66" s="148"/>
+      <c r="C66" s="146"/>
+      <c r="D66" s="147"/>
+      <c r="E66" s="148"/>
       <c r="F66" s="49"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="145"/>
-      <c r="B67" s="147"/>
-      <c r="C67" s="145"/>
-      <c r="D67" s="146"/>
-      <c r="E67" s="147"/>
+      <c r="A67" s="146"/>
+      <c r="B67" s="148"/>
+      <c r="C67" s="146"/>
+      <c r="D67" s="147"/>
+      <c r="E67" s="148"/>
       <c r="F67" s="49"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="145"/>
-      <c r="B68" s="147"/>
-      <c r="C68" s="145"/>
-      <c r="D68" s="146"/>
-      <c r="E68" s="147"/>
+      <c r="A68" s="146"/>
+      <c r="B68" s="148"/>
+      <c r="C68" s="146"/>
+      <c r="D68" s="147"/>
+      <c r="E68" s="148"/>
       <c r="F68" s="49"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="145"/>
-      <c r="B69" s="147"/>
-      <c r="C69" s="145"/>
-      <c r="D69" s="146"/>
-      <c r="E69" s="147"/>
+      <c r="A69" s="146"/>
+      <c r="B69" s="148"/>
+      <c r="C69" s="146"/>
+      <c r="D69" s="147"/>
+      <c r="E69" s="148"/>
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="148"/>
-      <c r="B70" s="150"/>
-      <c r="C70" s="148"/>
-      <c r="D70" s="149"/>
-      <c r="E70" s="150"/>
+      <c r="A70" s="149"/>
+      <c r="B70" s="151"/>
+      <c r="C70" s="149"/>
+      <c r="D70" s="150"/>
+      <c r="E70" s="151"/>
       <c r="F70" s="50"/>
     </row>
   </sheetData>
@@ -5409,10 +5435,10 @@
         <v>91</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="138" t="s">
+      <c r="C14" s="139" t="s">
         <v>179</v>
       </c>
-      <c r="D14" s="138"/>
+      <c r="D14" s="139"/>
       <c r="E14" s="54"/>
       <c r="F14" s="54"/>
       <c r="G14" s="54"/>
@@ -5426,10 +5452,10 @@
         <v>136</v>
       </c>
       <c r="B15" s="121"/>
-      <c r="C15" s="139" t="s">
+      <c r="C15" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="D15" s="139"/>
+      <c r="D15" s="140"/>
       <c r="E15" s="95" t="s">
         <v>137</v>
       </c>
@@ -5444,8 +5470,8 @@
         <v>138</v>
       </c>
       <c r="B16" s="121"/>
-      <c r="C16" s="140"/>
-      <c r="D16" s="139"/>
+      <c r="C16" s="141"/>
+      <c r="D16" s="140"/>
       <c r="E16" s="55" t="s">
         <v>175</v>
       </c>
@@ -5495,15 +5521,15 @@
       <c r="L18"/>
     </row>
     <row r="19" spans="1:22">
-      <c r="A19" s="177" t="s">
+      <c r="A19" s="178" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="177"/>
-      <c r="C19" s="177"/>
-      <c r="D19" s="177"/>
-      <c r="E19" s="177"/>
-      <c r="F19" s="177"/>
-      <c r="G19" s="177"/>
+      <c r="B19" s="178"/>
+      <c r="C19" s="178"/>
+      <c r="D19" s="178"/>
+      <c r="E19" s="178"/>
+      <c r="F19" s="178"/>
+      <c r="G19" s="178"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -5513,14 +5539,14 @@
       <c r="A20" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="171" t="s">
+      <c r="B20" s="172" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="172"/>
-      <c r="D20" s="172"/>
-      <c r="E20" s="172"/>
-      <c r="F20" s="172"/>
-      <c r="G20" s="173"/>
+      <c r="C20" s="173"/>
+      <c r="D20" s="173"/>
+      <c r="E20" s="173"/>
+      <c r="F20" s="173"/>
+      <c r="G20" s="174"/>
       <c r="H20" s="105"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -5538,12 +5564,12 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="116"/>
-      <c r="B21" s="160"/>
-      <c r="C21" s="160"/>
-      <c r="D21" s="160"/>
-      <c r="E21" s="160"/>
-      <c r="F21" s="160"/>
-      <c r="G21" s="160"/>
+      <c r="B21" s="161"/>
+      <c r="C21" s="161"/>
+      <c r="D21" s="161"/>
+      <c r="E21" s="161"/>
+      <c r="F21" s="161"/>
+      <c r="G21" s="161"/>
       <c r="H21" s="112"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -5561,12 +5587,12 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="117"/>
-      <c r="B22" s="156"/>
-      <c r="C22" s="156"/>
-      <c r="D22" s="156"/>
-      <c r="E22" s="156"/>
-      <c r="F22" s="156"/>
-      <c r="G22" s="156"/>
+      <c r="B22" s="157"/>
+      <c r="C22" s="157"/>
+      <c r="D22" s="157"/>
+      <c r="E22" s="157"/>
+      <c r="F22" s="157"/>
+      <c r="G22" s="157"/>
       <c r="H22" s="112"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -5584,12 +5610,12 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="118"/>
-      <c r="B23" s="158"/>
-      <c r="C23" s="158"/>
-      <c r="D23" s="158"/>
-      <c r="E23" s="158"/>
-      <c r="F23" s="158"/>
-      <c r="G23" s="158"/>
+      <c r="B23" s="159"/>
+      <c r="C23" s="159"/>
+      <c r="D23" s="159"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
       <c r="H23" s="112"/>
       <c r="M23" s="112"/>
       <c r="N23" s="112"/>
@@ -5609,15 +5635,15 @@
       <c r="L24" s="105"/>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="174" t="s">
+      <c r="A25" s="175" t="s">
         <v>152</v>
       </c>
-      <c r="B25" s="175"/>
-      <c r="C25" s="175"/>
-      <c r="D25" s="175"/>
-      <c r="E25" s="175"/>
-      <c r="F25" s="175"/>
-      <c r="G25" s="176"/>
+      <c r="B25" s="176"/>
+      <c r="C25" s="176"/>
+      <c r="D25" s="176"/>
+      <c r="E25" s="176"/>
+      <c r="F25" s="176"/>
+      <c r="G25" s="177"/>
       <c r="I25" s="105"/>
       <c r="J25" s="105"/>
       <c r="K25" s="105"/>
@@ -5627,14 +5653,14 @@
       <c r="A26" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="151" t="s">
+      <c r="B26" s="152" t="s">
         <v>144</v>
       </c>
-      <c r="C26" s="151"/>
-      <c r="D26" s="151"/>
-      <c r="E26" s="151"/>
-      <c r="F26" s="151"/>
-      <c r="G26" s="151"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="152"/>
+      <c r="G26" s="152"/>
       <c r="H26" s="105"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -5652,12 +5678,12 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="116"/>
-      <c r="B27" s="152"/>
-      <c r="C27" s="152"/>
-      <c r="D27" s="152"/>
-      <c r="E27" s="152"/>
-      <c r="F27" s="152"/>
-      <c r="G27" s="152"/>
+      <c r="B27" s="153"/>
+      <c r="C27" s="153"/>
+      <c r="D27" s="153"/>
+      <c r="E27" s="153"/>
+      <c r="F27" s="153"/>
+      <c r="G27" s="153"/>
       <c r="H27" s="112"/>
       <c r="I27"/>
       <c r="J27"/>
@@ -5675,12 +5701,12 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="117"/>
-      <c r="B28" s="153"/>
-      <c r="C28" s="153"/>
-      <c r="D28" s="153"/>
-      <c r="E28" s="153"/>
-      <c r="F28" s="153"/>
-      <c r="G28" s="153"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="154"/>
+      <c r="D28" s="154"/>
+      <c r="E28" s="154"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="154"/>
       <c r="H28" s="112"/>
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
@@ -5694,12 +5720,12 @@
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="118"/>
-      <c r="B29" s="154"/>
-      <c r="C29" s="154"/>
-      <c r="D29" s="154"/>
-      <c r="E29" s="154"/>
-      <c r="F29" s="154"/>
-      <c r="G29" s="154"/>
+      <c r="B29" s="155"/>
+      <c r="C29" s="155"/>
+      <c r="D29" s="155"/>
+      <c r="E29" s="155"/>
+      <c r="F29" s="155"/>
+      <c r="G29" s="155"/>
       <c r="H29" s="112"/>
       <c r="I29" s="105"/>
       <c r="J29" s="105"/>
@@ -5738,15 +5764,15 @@
       <c r="T30"/>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="174" t="s">
+      <c r="A31" s="175" t="s">
         <v>153</v>
       </c>
-      <c r="B31" s="175"/>
-      <c r="C31" s="175"/>
-      <c r="D31" s="175"/>
-      <c r="E31" s="175"/>
-      <c r="F31" s="175"/>
-      <c r="G31" s="176"/>
+      <c r="B31" s="176"/>
+      <c r="C31" s="176"/>
+      <c r="D31" s="176"/>
+      <c r="E31" s="176"/>
+      <c r="F31" s="176"/>
+      <c r="G31" s="177"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
       <c r="K31" s="112"/>
@@ -5756,14 +5782,14 @@
       <c r="A32" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="151" t="s">
+      <c r="B32" s="152" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="151"/>
-      <c r="D32" s="151"/>
-      <c r="E32" s="151"/>
-      <c r="F32" s="151"/>
-      <c r="G32" s="151"/>
+      <c r="C32" s="152"/>
+      <c r="D32" s="152"/>
+      <c r="E32" s="152"/>
+      <c r="F32" s="152"/>
+      <c r="G32" s="152"/>
       <c r="H32" s="105"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -5781,12 +5807,12 @@
     </row>
     <row r="33" spans="1:26">
       <c r="A33" s="116"/>
-      <c r="B33" s="160"/>
-      <c r="C33" s="160"/>
-      <c r="D33" s="160"/>
-      <c r="E33" s="160"/>
-      <c r="F33" s="160"/>
-      <c r="G33" s="196"/>
+      <c r="B33" s="161"/>
+      <c r="C33" s="161"/>
+      <c r="D33" s="161"/>
+      <c r="E33" s="161"/>
+      <c r="F33" s="161"/>
+      <c r="G33" s="197"/>
       <c r="H33" s="112"/>
       <c r="I33"/>
       <c r="J33"/>
@@ -5804,12 +5830,12 @@
     </row>
     <row r="34" spans="1:26">
       <c r="A34" s="117"/>
-      <c r="B34" s="156"/>
-      <c r="C34" s="156"/>
-      <c r="D34" s="156"/>
-      <c r="E34" s="156"/>
-      <c r="F34" s="156"/>
-      <c r="G34" s="157"/>
+      <c r="B34" s="157"/>
+      <c r="C34" s="157"/>
+      <c r="D34" s="157"/>
+      <c r="E34" s="157"/>
+      <c r="F34" s="157"/>
+      <c r="G34" s="158"/>
       <c r="H34" s="112"/>
       <c r="M34" s="112"/>
       <c r="N34" s="112"/>
@@ -5823,12 +5849,12 @@
     </row>
     <row r="35" spans="1:26">
       <c r="A35" s="118"/>
-      <c r="B35" s="158"/>
-      <c r="C35" s="158"/>
-      <c r="D35" s="158"/>
-      <c r="E35" s="158"/>
-      <c r="F35" s="158"/>
-      <c r="G35" s="159"/>
+      <c r="B35" s="159"/>
+      <c r="C35" s="159"/>
+      <c r="D35" s="159"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
+      <c r="G35" s="160"/>
       <c r="H35" s="112"/>
       <c r="M35" s="112"/>
       <c r="N35" s="112"/>
@@ -5892,82 +5918,82 @@
       <c r="Z38" s="39"/>
     </row>
     <row r="39" spans="1:26">
-      <c r="A39" s="184" t="s">
+      <c r="A39" s="185" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="184" t="s">
+      <c r="B39" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="186" t="s">
+      <c r="C39" s="187" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="184" t="s">
+      <c r="D39" s="185" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="187" t="s">
+      <c r="E39" s="188" t="s">
         <v>132</v>
       </c>
-      <c r="F39" s="187" t="s">
+      <c r="F39" s="188" t="s">
         <v>138</v>
       </c>
-      <c r="G39" s="184" t="s">
+      <c r="G39" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="H39" s="184" t="s">
+      <c r="H39" s="185" t="s">
         <v>95</v>
       </c>
-      <c r="I39" s="191" t="s">
+      <c r="I39" s="192" t="s">
         <v>158</v>
       </c>
-      <c r="J39" s="191" t="s">
+      <c r="J39" s="192" t="s">
         <v>159</v>
       </c>
-      <c r="K39" s="191" t="s">
+      <c r="K39" s="192" t="s">
         <v>160</v>
       </c>
-      <c r="L39" s="192" t="s">
+      <c r="L39" s="193" t="s">
         <v>161</v>
       </c>
-      <c r="M39" s="184" t="s">
+      <c r="M39" s="185" t="s">
         <v>154</v>
       </c>
-      <c r="N39" s="184" t="s">
+      <c r="N39" s="185" t="s">
         <v>164</v>
       </c>
-      <c r="O39" s="186" t="s">
+      <c r="O39" s="187" t="s">
         <v>163</v>
       </c>
-      <c r="P39" s="194" t="s">
+      <c r="P39" s="195" t="s">
         <v>71</v>
       </c>
-      <c r="Q39" s="195"/>
-      <c r="R39" s="194" t="s">
+      <c r="Q39" s="196"/>
+      <c r="R39" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="S39" s="195"/>
+      <c r="S39" s="196"/>
       <c r="T39" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="U39" s="184" t="s">
+      <c r="U39" s="185" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:26">
-      <c r="A40" s="185"/>
-      <c r="B40" s="185"/>
-      <c r="C40" s="185"/>
-      <c r="D40" s="185"/>
-      <c r="E40" s="188"/>
-      <c r="F40" s="189"/>
-      <c r="G40" s="185"/>
-      <c r="H40" s="185"/>
-      <c r="I40" s="191"/>
-      <c r="J40" s="191"/>
-      <c r="K40" s="191"/>
-      <c r="L40" s="193"/>
-      <c r="M40" s="190"/>
-      <c r="N40" s="190"/>
-      <c r="O40" s="190"/>
+      <c r="A40" s="186"/>
+      <c r="B40" s="186"/>
+      <c r="C40" s="186"/>
+      <c r="D40" s="186"/>
+      <c r="E40" s="189"/>
+      <c r="F40" s="190"/>
+      <c r="G40" s="186"/>
+      <c r="H40" s="186"/>
+      <c r="I40" s="192"/>
+      <c r="J40" s="192"/>
+      <c r="K40" s="192"/>
+      <c r="L40" s="194"/>
+      <c r="M40" s="191"/>
+      <c r="N40" s="191"/>
+      <c r="O40" s="191"/>
       <c r="P40" s="29" t="s">
         <v>75</v>
       </c>
@@ -5983,7 +6009,7 @@
       <c r="T40" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="U40" s="185"/>
+      <c r="U40" s="186"/>
     </row>
     <row r="41" spans="1:26" ht="45">
       <c r="A41" s="7">
@@ -6014,7 +6040,7 @@
       <c r="J41" s="132" t="s">
         <v>187</v>
       </c>
-      <c r="K41" s="206" t="s">
+      <c r="K41" s="137" t="s">
         <v>188</v>
       </c>
       <c r="L41" s="132" t="s">
@@ -6666,8 +6692,8 @@
   </sheetPr>
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -6842,10 +6868,10 @@
         <v>136</v>
       </c>
       <c r="B12" s="121"/>
-      <c r="C12" s="139" t="s">
+      <c r="C12" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="D12" s="139"/>
+      <c r="D12" s="140"/>
       <c r="E12" s="95" t="s">
         <v>137</v>
       </c>
@@ -6860,8 +6886,8 @@
         <v>138</v>
       </c>
       <c r="B13" s="121"/>
-      <c r="C13" s="139"/>
-      <c r="D13" s="139"/>
+      <c r="C13" s="140"/>
+      <c r="D13" s="140"/>
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="54"/>
@@ -6901,15 +6927,15 @@
       <c r="L15"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="177" t="s">
+      <c r="A16" s="178" t="s">
         <v>151</v>
       </c>
-      <c r="B16" s="177"/>
-      <c r="C16" s="177"/>
-      <c r="D16" s="177"/>
-      <c r="E16" s="177"/>
-      <c r="F16" s="177"/>
-      <c r="G16" s="177"/>
+      <c r="B16" s="178"/>
+      <c r="C16" s="178"/>
+      <c r="D16" s="178"/>
+      <c r="E16" s="178"/>
+      <c r="F16" s="178"/>
+      <c r="G16" s="178"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -6920,14 +6946,14 @@
       <c r="A17" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="172" t="s">
         <v>143</v>
       </c>
-      <c r="C17" s="172"/>
-      <c r="D17" s="172"/>
-      <c r="E17" s="172"/>
-      <c r="F17" s="172"/>
-      <c r="G17" s="173"/>
+      <c r="C17" s="173"/>
+      <c r="D17" s="173"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="174"/>
       <c r="H17" s="105"/>
       <c r="I17"/>
       <c r="J17"/>
@@ -6943,12 +6969,12 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="116"/>
-      <c r="B18" s="160"/>
-      <c r="C18" s="160"/>
-      <c r="D18" s="160"/>
-      <c r="E18" s="160"/>
-      <c r="F18" s="160"/>
-      <c r="G18" s="160"/>
+      <c r="B18" s="161"/>
+      <c r="C18" s="161"/>
+      <c r="D18" s="161"/>
+      <c r="E18" s="161"/>
+      <c r="F18" s="161"/>
+      <c r="G18" s="161"/>
       <c r="H18" s="112"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -6963,12 +6989,12 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="117"/>
-      <c r="B19" s="156"/>
-      <c r="C19" s="156"/>
-      <c r="D19" s="156"/>
-      <c r="E19" s="156"/>
-      <c r="F19" s="156"/>
-      <c r="G19" s="156"/>
+      <c r="B19" s="157"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="157"/>
+      <c r="E19" s="157"/>
+      <c r="F19" s="157"/>
+      <c r="G19" s="157"/>
       <c r="H19" s="112"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -6983,12 +7009,12 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="118"/>
-      <c r="B20" s="158"/>
-      <c r="C20" s="158"/>
-      <c r="D20" s="158"/>
-      <c r="E20" s="158"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="158"/>
+      <c r="B20" s="159"/>
+      <c r="C20" s="159"/>
+      <c r="D20" s="159"/>
+      <c r="E20" s="159"/>
+      <c r="F20" s="159"/>
+      <c r="G20" s="159"/>
       <c r="H20" s="112"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -7015,15 +7041,15 @@
       <c r="O21" s="112"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="174" t="s">
+      <c r="A22" s="175" t="s">
         <v>152</v>
       </c>
-      <c r="B22" s="175"/>
-      <c r="C22" s="175"/>
-      <c r="D22" s="175"/>
-      <c r="E22" s="175"/>
-      <c r="F22" s="175"/>
-      <c r="G22" s="176"/>
+      <c r="B22" s="176"/>
+      <c r="C22" s="176"/>
+      <c r="D22" s="176"/>
+      <c r="E22" s="176"/>
+      <c r="F22" s="176"/>
+      <c r="G22" s="177"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -7036,14 +7062,14 @@
       <c r="A23" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="151" t="s">
+      <c r="B23" s="152" t="s">
         <v>144</v>
       </c>
-      <c r="C23" s="151"/>
-      <c r="D23" s="151"/>
-      <c r="E23" s="151"/>
-      <c r="F23" s="151"/>
-      <c r="G23" s="151"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
       <c r="H23" s="105"/>
       <c r="M23" s="112"/>
       <c r="N23" s="112"/>
@@ -7057,12 +7083,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="116"/>
-      <c r="B24" s="152"/>
-      <c r="C24" s="152"/>
-      <c r="D24" s="152"/>
-      <c r="E24" s="152"/>
-      <c r="F24" s="152"/>
-      <c r="G24" s="152"/>
+      <c r="B24" s="153"/>
+      <c r="C24" s="153"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="153"/>
+      <c r="F24" s="153"/>
+      <c r="G24" s="153"/>
       <c r="H24" s="112"/>
       <c r="I24" s="105"/>
       <c r="J24" s="105"/>
@@ -7077,12 +7103,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="117"/>
-      <c r="B25" s="153"/>
-      <c r="C25" s="153"/>
-      <c r="D25" s="153"/>
-      <c r="E25" s="153"/>
-      <c r="F25" s="153"/>
-      <c r="G25" s="153"/>
+      <c r="B25" s="154"/>
+      <c r="C25" s="154"/>
+      <c r="D25" s="154"/>
+      <c r="E25" s="154"/>
+      <c r="F25" s="154"/>
+      <c r="G25" s="154"/>
       <c r="H25" s="112"/>
       <c r="I25" s="105"/>
       <c r="J25" s="105"/>
@@ -7097,12 +7123,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="118"/>
-      <c r="B26" s="154"/>
-      <c r="C26" s="154"/>
-      <c r="D26" s="154"/>
-      <c r="E26" s="154"/>
-      <c r="F26" s="154"/>
-      <c r="G26" s="154"/>
+      <c r="B26" s="155"/>
+      <c r="C26" s="155"/>
+      <c r="D26" s="155"/>
+      <c r="E26" s="155"/>
+      <c r="F26" s="155"/>
+      <c r="G26" s="155"/>
       <c r="H26" s="112"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -7141,15 +7167,15 @@
       <c r="T27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="174" t="s">
+      <c r="A28" s="175" t="s">
         <v>153</v>
       </c>
-      <c r="B28" s="175"/>
-      <c r="C28" s="175"/>
-      <c r="D28" s="175"/>
-      <c r="E28" s="175"/>
-      <c r="F28" s="175"/>
-      <c r="G28" s="176"/>
+      <c r="B28" s="176"/>
+      <c r="C28" s="176"/>
+      <c r="D28" s="176"/>
+      <c r="E28" s="176"/>
+      <c r="F28" s="176"/>
+      <c r="G28" s="177"/>
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
       <c r="O28" s="112"/>
@@ -7158,14 +7184,14 @@
       <c r="A29" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="151" t="s">
+      <c r="B29" s="152" t="s">
         <v>145</v>
       </c>
-      <c r="C29" s="151"/>
-      <c r="D29" s="151"/>
-      <c r="E29" s="151"/>
-      <c r="F29" s="151"/>
-      <c r="G29" s="151"/>
+      <c r="C29" s="152"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="152"/>
+      <c r="G29" s="152"/>
       <c r="H29" s="105"/>
       <c r="I29" s="105"/>
       <c r="J29" s="105"/>
@@ -7183,12 +7209,12 @@
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="116"/>
-      <c r="B30" s="160"/>
-      <c r="C30" s="160"/>
-      <c r="D30" s="160"/>
-      <c r="E30" s="160"/>
-      <c r="F30" s="160"/>
-      <c r="G30" s="196"/>
+      <c r="B30" s="161"/>
+      <c r="C30" s="161"/>
+      <c r="D30" s="161"/>
+      <c r="E30" s="161"/>
+      <c r="F30" s="161"/>
+      <c r="G30" s="197"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -7206,12 +7232,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="117"/>
-      <c r="B31" s="156"/>
-      <c r="C31" s="156"/>
-      <c r="D31" s="156"/>
-      <c r="E31" s="156"/>
-      <c r="F31" s="156"/>
-      <c r="G31" s="157"/>
+      <c r="B31" s="157"/>
+      <c r="C31" s="157"/>
+      <c r="D31" s="157"/>
+      <c r="E31" s="157"/>
+      <c r="F31" s="157"/>
+      <c r="G31" s="158"/>
       <c r="H31" s="112"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
@@ -7226,12 +7252,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="118"/>
-      <c r="B32" s="158"/>
-      <c r="C32" s="158"/>
-      <c r="D32" s="158"/>
-      <c r="E32" s="158"/>
-      <c r="F32" s="158"/>
-      <c r="G32" s="159"/>
+      <c r="B32" s="159"/>
+      <c r="C32" s="159"/>
+      <c r="D32" s="159"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="159"/>
+      <c r="G32" s="160"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -7301,84 +7327,84 @@
       <c r="U35" s="58"/>
     </row>
     <row r="36" spans="1:21" ht="30" customHeight="1">
-      <c r="A36" s="187" t="s">
+      <c r="A36" s="188" t="s">
         <v>97</v>
       </c>
-      <c r="B36" s="187" t="s">
+      <c r="B36" s="188" t="s">
         <v>98</v>
       </c>
       <c r="C36" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="187" t="s">
+      <c r="D36" s="188" t="s">
         <v>92</v>
       </c>
-      <c r="E36" s="187" t="s">
+      <c r="E36" s="188" t="s">
         <v>132</v>
       </c>
-      <c r="F36" s="187" t="s">
+      <c r="F36" s="188" t="s">
         <v>138</v>
       </c>
-      <c r="G36" s="187" t="s">
+      <c r="G36" s="188" t="s">
         <v>111</v>
       </c>
-      <c r="H36" s="187" t="s">
+      <c r="H36" s="188" t="s">
         <v>110</v>
       </c>
-      <c r="I36" s="202" t="s">
+      <c r="I36" s="203" t="s">
         <v>158</v>
       </c>
-      <c r="J36" s="204" t="s">
+      <c r="J36" s="205" t="s">
         <v>159</v>
       </c>
-      <c r="K36" s="204" t="s">
+      <c r="K36" s="205" t="s">
         <v>160</v>
       </c>
-      <c r="L36" s="192" t="s">
+      <c r="L36" s="193" t="s">
         <v>161</v>
       </c>
-      <c r="M36" s="184" t="s">
+      <c r="M36" s="185" t="s">
         <v>154</v>
       </c>
-      <c r="N36" s="184" t="s">
+      <c r="N36" s="185" t="s">
         <v>164</v>
       </c>
-      <c r="O36" s="186" t="s">
+      <c r="O36" s="187" t="s">
         <v>163</v>
       </c>
-      <c r="P36" s="201" t="s">
+      <c r="P36" s="202" t="s">
         <v>101</v>
       </c>
-      <c r="Q36" s="199"/>
-      <c r="R36" s="198" t="s">
+      <c r="Q36" s="200"/>
+      <c r="R36" s="199" t="s">
         <v>102</v>
       </c>
-      <c r="S36" s="199"/>
+      <c r="S36" s="200"/>
       <c r="T36" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="U36" s="187" t="s">
+      <c r="U36" s="188" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15">
-      <c r="A37" s="200"/>
-      <c r="B37" s="200"/>
+      <c r="A37" s="201"/>
+      <c r="B37" s="201"/>
       <c r="C37" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="D37" s="200"/>
-      <c r="E37" s="189"/>
-      <c r="F37" s="189"/>
-      <c r="G37" s="200"/>
-      <c r="H37" s="200"/>
-      <c r="I37" s="203"/>
-      <c r="J37" s="205"/>
-      <c r="K37" s="205"/>
-      <c r="L37" s="193"/>
-      <c r="M37" s="190"/>
-      <c r="N37" s="190"/>
-      <c r="O37" s="197"/>
+      <c r="D37" s="201"/>
+      <c r="E37" s="190"/>
+      <c r="F37" s="190"/>
+      <c r="G37" s="201"/>
+      <c r="H37" s="201"/>
+      <c r="I37" s="204"/>
+      <c r="J37" s="206"/>
+      <c r="K37" s="206"/>
+      <c r="L37" s="194"/>
+      <c r="M37" s="191"/>
+      <c r="N37" s="191"/>
+      <c r="O37" s="198"/>
       <c r="P37" s="62" t="s">
         <v>105</v>
       </c>
@@ -7394,7 +7420,7 @@
       <c r="T37" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="U37" s="200"/>
+      <c r="U37" s="201"/>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="64">
@@ -7446,10 +7472,18 @@
       <c r="U38" s="68"/>
     </row>
     <row r="39" spans="1:21" ht="14" customHeight="1">
-      <c r="A39" s="64"/>
-      <c r="B39" s="65"/>
-      <c r="C39" s="66"/>
-      <c r="D39" s="67"/>
+      <c r="A39" s="64">
+        <v>2</v>
+      </c>
+      <c r="B39" s="69" t="s">
+        <v>197</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" s="70" t="s">
+        <v>196</v>
+      </c>
       <c r="E39" s="67"/>
       <c r="F39" s="67"/>
       <c r="G39" s="89"/>
@@ -7469,11 +7503,21 @@
       <c r="U39" s="68"/>
     </row>
     <row r="40" spans="1:21">
-      <c r="A40" s="64"/>
-      <c r="B40" s="69"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="70"/>
-      <c r="E40" s="70"/>
+      <c r="A40" s="64">
+        <v>3</v>
+      </c>
+      <c r="B40" s="69" t="s">
+        <v>199</v>
+      </c>
+      <c r="C40" s="51" t="s">
+        <v>200</v>
+      </c>
+      <c r="D40" s="70" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" s="70" t="s">
+        <v>196</v>
+      </c>
       <c r="F40" s="70"/>
       <c r="G40" s="90"/>
       <c r="H40" s="70"/>

</xml_diff>

<commit_message>
0.0.7: fix bug on array parsing. * correct parsing terminator count. * parse empty cell as null. * no element array will be ignored.
</commit_message>
<xml_diff>
--- a/meta/api/GetTableSample2.xlsx
+++ b/meta/api/GetTableSample2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A223CE-05A1-9944-B228-775FD33AD02C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597F28B3-85E0-2542-9462-571179D5E290}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14540" yWindow="460" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,18 +21,17 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="isImport">config!$E$5:$E$6</definedName>
     <definedName name="isNullable">config!$F$5:$F$6</definedName>
     <definedName name="others">config!$G$5:$G$6</definedName>
     <definedName name="Submit有無">config!$B$5:$B$6</definedName>
-    <definedName name="threeAlters">[1]config!$H$5:$H$7</definedName>
+    <definedName name="threeAlters">config!$H$5:$H$7</definedName>
     <definedName name="Validate実装パターン">config!$A$5:$A$6</definedName>
     <definedName name="チェック種別">config!$D$5:$D$49</definedName>
     <definedName name="型">config!#REF!</definedName>
-    <definedName name="形式タイプ">[2]telegramConfig!$D$6:$D$27</definedName>
+    <definedName name="形式タイプ">[1]telegramConfig!$D$6:$D$27</definedName>
     <definedName name="項目型" localSheetId="1">config!#REF!</definedName>
     <definedName name="項目型" localSheetId="2">config!#REF!</definedName>
     <definedName name="項目型">config!#REF!</definedName>
@@ -3508,146 +3507,158 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="59" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3668,50 +3679,38 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3803,38 +3802,6 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="process"/>
-      <sheetName val="post_input"/>
-      <sheetName val="post_output"/>
-      <sheetName val="readme"/>
-      <sheetName val="config"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
-        <row r="5">
-          <cell r="H5" t="str">
-            <v>YES</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="H6" t="str">
-            <v>NOT</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -4335,137 +4302,137 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="138" t="s">
+      <c r="A5" s="184" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="138"/>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="138"/>
+      <c r="B5" s="184"/>
+      <c r="C5" s="184"/>
+      <c r="D5" s="184"/>
+      <c r="E5" s="184"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="95"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="142" t="s">
+      <c r="A6" s="181" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="143"/>
-      <c r="C6" s="144"/>
-      <c r="D6" s="139" t="s">
+      <c r="B6" s="182"/>
+      <c r="C6" s="183"/>
+      <c r="D6" s="180" t="s">
         <v>183</v>
       </c>
-      <c r="E6" s="139"/>
+      <c r="E6" s="180"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="138" t="s">
+      <c r="A7" s="184" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="138"/>
-      <c r="C7" s="138"/>
-      <c r="D7" s="139" t="s">
+      <c r="B7" s="184"/>
+      <c r="C7" s="184"/>
+      <c r="D7" s="180" t="s">
         <v>133</v>
       </c>
-      <c r="E7" s="139"/>
+      <c r="E7" s="180"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="138" t="s">
+      <c r="A8" s="184" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="138"/>
-      <c r="C8" s="138"/>
-      <c r="D8" s="139" t="s">
+      <c r="B8" s="184"/>
+      <c r="C8" s="184"/>
+      <c r="D8" s="180" t="s">
         <v>183</v>
       </c>
-      <c r="E8" s="139"/>
+      <c r="E8" s="180"/>
       <c r="F8" s="95"/>
       <c r="G8" s="95"/>
       <c r="H8" s="95"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="138" t="s">
+      <c r="A9" s="184" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="138"/>
-      <c r="C9" s="138"/>
-      <c r="D9" s="139" t="s">
+      <c r="B9" s="184"/>
+      <c r="C9" s="184"/>
+      <c r="D9" s="180" t="s">
         <v>180</v>
       </c>
-      <c r="E9" s="139"/>
+      <c r="E9" s="180"/>
       <c r="F9" s="95"/>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="138" t="s">
+      <c r="A10" s="184" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="138"/>
-      <c r="C10" s="138"/>
-      <c r="D10" s="139"/>
-      <c r="E10" s="139"/>
+      <c r="B10" s="184"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="180"/>
+      <c r="E10" s="180"/>
       <c r="F10" s="95"/>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="138" t="s">
+      <c r="A11" s="184" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="138"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="139" t="s">
+      <c r="B11" s="184"/>
+      <c r="C11" s="184"/>
+      <c r="D11" s="180" t="s">
         <v>179</v>
       </c>
-      <c r="E11" s="139"/>
+      <c r="E11" s="180"/>
       <c r="F11" s="95"/>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="145" t="s">
+      <c r="A12" s="143" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="145"/>
-      <c r="C12" s="145"/>
-      <c r="D12" s="140" t="s">
+      <c r="B12" s="143"/>
+      <c r="C12" s="143"/>
+      <c r="D12" s="164" t="s">
         <v>177</v>
       </c>
-      <c r="E12" s="140"/>
+      <c r="E12" s="164"/>
       <c r="F12" s="95" t="s">
         <v>137</v>
       </c>
       <c r="G12" s="54"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="145" t="s">
+      <c r="A13" s="143" t="s">
         <v>167</v>
       </c>
-      <c r="B13" s="145"/>
-      <c r="C13" s="145"/>
-      <c r="D13" s="140" t="s">
+      <c r="B13" s="143"/>
+      <c r="C13" s="143"/>
+      <c r="D13" s="164" t="s">
         <v>165</v>
       </c>
-      <c r="E13" s="140"/>
+      <c r="E13" s="164"/>
       <c r="F13" s="95" t="s">
         <v>166</v>
       </c>
       <c r="G13" s="54"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="145" t="s">
+      <c r="A14" s="143" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="145"/>
-      <c r="C14" s="145"/>
-      <c r="D14" s="141"/>
-      <c r="E14" s="140"/>
+      <c r="B14" s="143"/>
+      <c r="C14" s="143"/>
+      <c r="D14" s="163"/>
+      <c r="E14" s="164"/>
       <c r="F14" s="54" t="s">
         <v>156</v>
       </c>
@@ -4473,15 +4440,15 @@
       <c r="H14" s="95"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="145" t="s">
+      <c r="A15" s="143" t="s">
         <v>171</v>
       </c>
-      <c r="B15" s="145"/>
-      <c r="C15" s="145"/>
-      <c r="D15" s="141" t="s">
+      <c r="B15" s="143"/>
+      <c r="C15" s="143"/>
+      <c r="D15" s="163" t="s">
         <v>181</v>
       </c>
-      <c r="E15" s="140"/>
+      <c r="E15" s="164"/>
       <c r="F15" s="54" t="s">
         <v>173</v>
       </c>
@@ -4489,13 +4456,13 @@
       <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="145" t="s">
+      <c r="A16" s="143" t="s">
         <v>170</v>
       </c>
-      <c r="B16" s="145"/>
-      <c r="C16" s="145"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="140"/>
+      <c r="B16" s="143"/>
+      <c r="C16" s="143"/>
+      <c r="D16" s="163"/>
+      <c r="E16" s="164"/>
       <c r="F16" s="54" t="s">
         <v>172</v>
       </c>
@@ -4503,15 +4470,15 @@
       <c r="H16" s="95"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="145" t="s">
+      <c r="A17" s="143" t="s">
         <v>169</v>
       </c>
-      <c r="B17" s="145"/>
-      <c r="C17" s="145"/>
-      <c r="D17" s="141" t="s">
+      <c r="B17" s="143"/>
+      <c r="C17" s="143"/>
+      <c r="D17" s="163" t="s">
         <v>174</v>
       </c>
-      <c r="E17" s="140"/>
+      <c r="E17" s="164"/>
       <c r="F17" s="54" t="s">
         <v>168</v>
       </c>
@@ -4519,19 +4486,19 @@
       <c r="H17" s="95"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="182" t="s">
+      <c r="A18" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="183"/>
-      <c r="C18" s="184"/>
+      <c r="B18" s="161"/>
+      <c r="C18" s="162"/>
       <c r="D18" s="114"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="168" t="s">
+      <c r="A19" s="144" t="s">
         <v>139</v>
       </c>
-      <c r="B19" s="169"/>
-      <c r="C19" s="170"/>
+      <c r="B19" s="145"/>
+      <c r="C19" s="146"/>
       <c r="D19" s="100"/>
       <c r="E19" t="s">
         <v>140</v>
@@ -4549,15 +4516,15 @@
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="179" t="s">
+      <c r="A21" s="157" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="180"/>
-      <c r="C21" s="180"/>
-      <c r="D21" s="180"/>
-      <c r="E21" s="180"/>
-      <c r="F21" s="180"/>
-      <c r="G21" s="181"/>
+      <c r="B21" s="158"/>
+      <c r="C21" s="158"/>
+      <c r="D21" s="158"/>
+      <c r="E21" s="158"/>
+      <c r="F21" s="158"/>
+      <c r="G21" s="159"/>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="101" t="s">
@@ -4605,28 +4572,28 @@
       <c r="C25"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="178" t="s">
+      <c r="A26" s="156" t="s">
         <v>148</v>
       </c>
-      <c r="B26" s="178"/>
-      <c r="C26" s="178"/>
-      <c r="D26" s="178"/>
-      <c r="E26" s="178"/>
-      <c r="F26" s="178"/>
-      <c r="G26" s="178"/>
+      <c r="B26" s="156"/>
+      <c r="C26" s="156"/>
+      <c r="D26" s="156"/>
+      <c r="E26" s="156"/>
+      <c r="F26" s="156"/>
+      <c r="G26" s="156"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="172" t="s">
+      <c r="B27" s="150" t="s">
         <v>143</v>
       </c>
-      <c r="C27" s="173"/>
-      <c r="D27" s="173"/>
-      <c r="E27" s="173"/>
-      <c r="F27" s="173"/>
-      <c r="G27" s="174"/>
+      <c r="C27" s="151"/>
+      <c r="D27" s="151"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="151"/>
+      <c r="G27" s="152"/>
       <c r="H27" s="105"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -4637,12 +4604,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="116"/>
-      <c r="B28" s="161"/>
-      <c r="C28" s="161"/>
-      <c r="D28" s="161"/>
-      <c r="E28" s="161"/>
-      <c r="F28" s="161"/>
-      <c r="G28" s="161"/>
+      <c r="B28" s="167"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="167"/>
       <c r="H28" s="112"/>
       <c r="I28" s="112"/>
       <c r="J28" s="112"/>
@@ -4653,12 +4620,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="117"/>
-      <c r="B29" s="157"/>
-      <c r="C29" s="157"/>
-      <c r="D29" s="157"/>
-      <c r="E29" s="157"/>
-      <c r="F29" s="157"/>
-      <c r="G29" s="157"/>
+      <c r="B29" s="168"/>
+      <c r="C29" s="168"/>
+      <c r="D29" s="168"/>
+      <c r="E29" s="168"/>
+      <c r="F29" s="168"/>
+      <c r="G29" s="168"/>
       <c r="H29" s="112"/>
       <c r="I29" s="112"/>
       <c r="J29" s="112"/>
@@ -4669,12 +4636,12 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="118"/>
-      <c r="B30" s="159"/>
-      <c r="C30" s="159"/>
-      <c r="D30" s="159"/>
-      <c r="E30" s="159"/>
-      <c r="F30" s="159"/>
-      <c r="G30" s="159"/>
+      <c r="B30" s="169"/>
+      <c r="C30" s="169"/>
+      <c r="D30" s="169"/>
+      <c r="E30" s="169"/>
+      <c r="F30" s="169"/>
+      <c r="G30" s="169"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -4687,28 +4654,28 @@
       <c r="C31"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="175" t="s">
+      <c r="A32" s="153" t="s">
         <v>149</v>
       </c>
-      <c r="B32" s="176"/>
-      <c r="C32" s="176"/>
-      <c r="D32" s="176"/>
-      <c r="E32" s="176"/>
-      <c r="F32" s="176"/>
-      <c r="G32" s="177"/>
+      <c r="B32" s="154"/>
+      <c r="C32" s="154"/>
+      <c r="D32" s="154"/>
+      <c r="E32" s="154"/>
+      <c r="F32" s="154"/>
+      <c r="G32" s="155"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="152" t="s">
+      <c r="B33" s="173" t="s">
         <v>144</v>
       </c>
-      <c r="C33" s="152"/>
-      <c r="D33" s="152"/>
-      <c r="E33" s="152"/>
-      <c r="F33" s="152"/>
-      <c r="G33" s="152"/>
+      <c r="C33" s="173"/>
+      <c r="D33" s="173"/>
+      <c r="E33" s="173"/>
+      <c r="F33" s="173"/>
+      <c r="G33" s="173"/>
       <c r="H33" s="105"/>
       <c r="I33" s="105"/>
       <c r="J33" s="105"/>
@@ -4719,12 +4686,12 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="116"/>
-      <c r="B34" s="153"/>
-      <c r="C34" s="153"/>
-      <c r="D34" s="153"/>
-      <c r="E34" s="153"/>
-      <c r="F34" s="153"/>
-      <c r="G34" s="153"/>
+      <c r="B34" s="174"/>
+      <c r="C34" s="174"/>
+      <c r="D34" s="174"/>
+      <c r="E34" s="174"/>
+      <c r="F34" s="174"/>
+      <c r="G34" s="174"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -4735,12 +4702,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="117"/>
-      <c r="B35" s="154"/>
-      <c r="C35" s="154"/>
-      <c r="D35" s="154"/>
-      <c r="E35" s="154"/>
-      <c r="F35" s="154"/>
-      <c r="G35" s="154"/>
+      <c r="B35" s="175"/>
+      <c r="C35" s="175"/>
+      <c r="D35" s="175"/>
+      <c r="E35" s="175"/>
+      <c r="F35" s="175"/>
+      <c r="G35" s="175"/>
       <c r="H35" s="112"/>
       <c r="I35" s="112"/>
       <c r="J35" s="112"/>
@@ -4751,12 +4718,12 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="118"/>
-      <c r="B36" s="155"/>
-      <c r="C36" s="155"/>
-      <c r="D36" s="155"/>
-      <c r="E36" s="155"/>
-      <c r="F36" s="155"/>
-      <c r="G36" s="155"/>
+      <c r="B36" s="176"/>
+      <c r="C36" s="176"/>
+      <c r="D36" s="176"/>
+      <c r="E36" s="176"/>
+      <c r="F36" s="176"/>
+      <c r="G36" s="176"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -4781,28 +4748,28 @@
       <c r="M37"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="175" t="s">
+      <c r="A38" s="153" t="s">
         <v>150</v>
       </c>
-      <c r="B38" s="176"/>
-      <c r="C38" s="176"/>
-      <c r="D38" s="176"/>
-      <c r="E38" s="176"/>
-      <c r="F38" s="176"/>
-      <c r="G38" s="177"/>
+      <c r="B38" s="154"/>
+      <c r="C38" s="154"/>
+      <c r="D38" s="154"/>
+      <c r="E38" s="154"/>
+      <c r="F38" s="154"/>
+      <c r="G38" s="155"/>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="152" t="s">
+      <c r="B39" s="173" t="s">
         <v>145</v>
       </c>
-      <c r="C39" s="152"/>
-      <c r="D39" s="152"/>
-      <c r="E39" s="152"/>
-      <c r="F39" s="152"/>
-      <c r="G39" s="152"/>
+      <c r="C39" s="173"/>
+      <c r="D39" s="173"/>
+      <c r="E39" s="173"/>
+      <c r="F39" s="173"/>
+      <c r="G39" s="173"/>
       <c r="H39" s="105"/>
       <c r="I39" s="105"/>
       <c r="J39" s="105"/>
@@ -4813,12 +4780,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="116"/>
-      <c r="B40" s="153"/>
-      <c r="C40" s="153"/>
-      <c r="D40" s="153"/>
-      <c r="E40" s="153"/>
-      <c r="F40" s="153"/>
-      <c r="G40" s="156"/>
+      <c r="B40" s="174"/>
+      <c r="C40" s="174"/>
+      <c r="D40" s="174"/>
+      <c r="E40" s="174"/>
+      <c r="F40" s="174"/>
+      <c r="G40" s="177"/>
       <c r="H40" s="112"/>
       <c r="I40" s="112"/>
       <c r="J40" s="112"/>
@@ -4829,12 +4796,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="117"/>
-      <c r="B41" s="157"/>
-      <c r="C41" s="157"/>
-      <c r="D41" s="157"/>
-      <c r="E41" s="157"/>
-      <c r="F41" s="157"/>
-      <c r="G41" s="158"/>
+      <c r="B41" s="168"/>
+      <c r="C41" s="168"/>
+      <c r="D41" s="168"/>
+      <c r="E41" s="168"/>
+      <c r="F41" s="168"/>
+      <c r="G41" s="178"/>
       <c r="H41" s="112"/>
       <c r="I41" s="112"/>
       <c r="J41" s="112"/>
@@ -4845,12 +4812,12 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="118"/>
-      <c r="B42" s="159"/>
-      <c r="C42" s="159"/>
-      <c r="D42" s="159"/>
-      <c r="E42" s="159"/>
-      <c r="F42" s="159"/>
-      <c r="G42" s="160"/>
+      <c r="B42" s="169"/>
+      <c r="C42" s="169"/>
+      <c r="D42" s="169"/>
+      <c r="E42" s="169"/>
+      <c r="F42" s="169"/>
+      <c r="G42" s="179"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -4885,254 +4852,267 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="165" t="s">
+      <c r="A45" s="140" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="171"/>
-      <c r="C45" s="165" t="s">
+      <c r="B45" s="147"/>
+      <c r="C45" s="140" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="166"/>
-      <c r="E45" s="167"/>
+      <c r="D45" s="141"/>
+      <c r="E45" s="142"/>
       <c r="F45" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="162"/>
-      <c r="B46" s="164"/>
-      <c r="C46" s="162"/>
-      <c r="D46" s="163"/>
-      <c r="E46" s="164"/>
+      <c r="A46" s="148"/>
+      <c r="B46" s="149"/>
+      <c r="C46" s="148"/>
+      <c r="D46" s="170"/>
+      <c r="E46" s="149"/>
       <c r="F46" s="49"/>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="146"/>
-      <c r="B47" s="148"/>
-      <c r="C47" s="146"/>
-      <c r="D47" s="147"/>
-      <c r="E47" s="148"/>
+      <c r="A47" s="138"/>
+      <c r="B47" s="139"/>
+      <c r="C47" s="138"/>
+      <c r="D47" s="171"/>
+      <c r="E47" s="139"/>
       <c r="F47" s="49"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="146"/>
-      <c r="B48" s="148"/>
-      <c r="C48" s="146"/>
-      <c r="D48" s="147"/>
-      <c r="E48" s="148"/>
+      <c r="A48" s="138"/>
+      <c r="B48" s="139"/>
+      <c r="C48" s="138"/>
+      <c r="D48" s="171"/>
+      <c r="E48" s="139"/>
       <c r="F48" s="49"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="146"/>
-      <c r="B49" s="148"/>
-      <c r="C49" s="146"/>
-      <c r="D49" s="147"/>
-      <c r="E49" s="148"/>
+      <c r="A49" s="138"/>
+      <c r="B49" s="139"/>
+      <c r="C49" s="138"/>
+      <c r="D49" s="171"/>
+      <c r="E49" s="139"/>
       <c r="F49" s="49"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="146"/>
-      <c r="B50" s="148"/>
-      <c r="C50" s="146"/>
-      <c r="D50" s="147"/>
-      <c r="E50" s="148"/>
+      <c r="A50" s="138"/>
+      <c r="B50" s="139"/>
+      <c r="C50" s="138"/>
+      <c r="D50" s="171"/>
+      <c r="E50" s="139"/>
       <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="146"/>
-      <c r="B51" s="148"/>
-      <c r="C51" s="146"/>
-      <c r="D51" s="147"/>
-      <c r="E51" s="148"/>
+      <c r="A51" s="138"/>
+      <c r="B51" s="139"/>
+      <c r="C51" s="138"/>
+      <c r="D51" s="171"/>
+      <c r="E51" s="139"/>
       <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="146"/>
-      <c r="B52" s="148"/>
-      <c r="C52" s="146"/>
-      <c r="D52" s="147"/>
-      <c r="E52" s="148"/>
+      <c r="A52" s="138"/>
+      <c r="B52" s="139"/>
+      <c r="C52" s="138"/>
+      <c r="D52" s="171"/>
+      <c r="E52" s="139"/>
       <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="146"/>
-      <c r="B53" s="148"/>
-      <c r="C53" s="146"/>
-      <c r="D53" s="147"/>
-      <c r="E53" s="148"/>
+      <c r="A53" s="138"/>
+      <c r="B53" s="139"/>
+      <c r="C53" s="138"/>
+      <c r="D53" s="171"/>
+      <c r="E53" s="139"/>
       <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="146"/>
-      <c r="B54" s="148"/>
-      <c r="C54" s="146"/>
-      <c r="D54" s="147"/>
-      <c r="E54" s="148"/>
+      <c r="A54" s="138"/>
+      <c r="B54" s="139"/>
+      <c r="C54" s="138"/>
+      <c r="D54" s="171"/>
+      <c r="E54" s="139"/>
       <c r="F54" s="49"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="146"/>
-      <c r="B55" s="148"/>
-      <c r="C55" s="146"/>
-      <c r="D55" s="147"/>
-      <c r="E55" s="148"/>
+      <c r="A55" s="138"/>
+      <c r="B55" s="139"/>
+      <c r="C55" s="138"/>
+      <c r="D55" s="171"/>
+      <c r="E55" s="139"/>
       <c r="F55" s="49"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="146"/>
-      <c r="B56" s="148"/>
-      <c r="C56" s="146"/>
-      <c r="D56" s="147"/>
-      <c r="E56" s="148"/>
+      <c r="A56" s="138"/>
+      <c r="B56" s="139"/>
+      <c r="C56" s="138"/>
+      <c r="D56" s="171"/>
+      <c r="E56" s="139"/>
       <c r="F56" s="49"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="146"/>
-      <c r="B57" s="148"/>
-      <c r="C57" s="146"/>
-      <c r="D57" s="147"/>
-      <c r="E57" s="148"/>
+      <c r="A57" s="138"/>
+      <c r="B57" s="139"/>
+      <c r="C57" s="138"/>
+      <c r="D57" s="171"/>
+      <c r="E57" s="139"/>
       <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="146"/>
-      <c r="B58" s="148"/>
-      <c r="C58" s="146"/>
-      <c r="D58" s="147"/>
-      <c r="E58" s="148"/>
+      <c r="A58" s="138"/>
+      <c r="B58" s="139"/>
+      <c r="C58" s="138"/>
+      <c r="D58" s="171"/>
+      <c r="E58" s="139"/>
       <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="146"/>
-      <c r="B59" s="148"/>
-      <c r="C59" s="146"/>
-      <c r="D59" s="147"/>
-      <c r="E59" s="148"/>
+      <c r="A59" s="138"/>
+      <c r="B59" s="139"/>
+      <c r="C59" s="138"/>
+      <c r="D59" s="171"/>
+      <c r="E59" s="139"/>
       <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="146"/>
-      <c r="B60" s="148"/>
-      <c r="C60" s="146"/>
-      <c r="D60" s="147"/>
-      <c r="E60" s="148"/>
+      <c r="A60" s="138"/>
+      <c r="B60" s="139"/>
+      <c r="C60" s="138"/>
+      <c r="D60" s="171"/>
+      <c r="E60" s="139"/>
       <c r="F60" s="49"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="146"/>
-      <c r="B61" s="148"/>
-      <c r="C61" s="146"/>
-      <c r="D61" s="147"/>
-      <c r="E61" s="148"/>
+      <c r="A61" s="138"/>
+      <c r="B61" s="139"/>
+      <c r="C61" s="138"/>
+      <c r="D61" s="171"/>
+      <c r="E61" s="139"/>
       <c r="F61" s="49"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="146"/>
-      <c r="B62" s="148"/>
-      <c r="C62" s="146"/>
-      <c r="D62" s="147"/>
-      <c r="E62" s="148"/>
+      <c r="A62" s="138"/>
+      <c r="B62" s="139"/>
+      <c r="C62" s="138"/>
+      <c r="D62" s="171"/>
+      <c r="E62" s="139"/>
       <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="146"/>
-      <c r="B63" s="148"/>
-      <c r="C63" s="146"/>
-      <c r="D63" s="147"/>
-      <c r="E63" s="148"/>
+      <c r="A63" s="138"/>
+      <c r="B63" s="139"/>
+      <c r="C63" s="138"/>
+      <c r="D63" s="171"/>
+      <c r="E63" s="139"/>
       <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="146"/>
-      <c r="B64" s="148"/>
-      <c r="C64" s="146"/>
-      <c r="D64" s="147"/>
-      <c r="E64" s="148"/>
+      <c r="A64" s="138"/>
+      <c r="B64" s="139"/>
+      <c r="C64" s="138"/>
+      <c r="D64" s="171"/>
+      <c r="E64" s="139"/>
       <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="146"/>
-      <c r="B65" s="148"/>
-      <c r="C65" s="146"/>
-      <c r="D65" s="147"/>
-      <c r="E65" s="148"/>
+      <c r="A65" s="138"/>
+      <c r="B65" s="139"/>
+      <c r="C65" s="138"/>
+      <c r="D65" s="171"/>
+      <c r="E65" s="139"/>
       <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="146"/>
-      <c r="B66" s="148"/>
-      <c r="C66" s="146"/>
-      <c r="D66" s="147"/>
-      <c r="E66" s="148"/>
+      <c r="A66" s="138"/>
+      <c r="B66" s="139"/>
+      <c r="C66" s="138"/>
+      <c r="D66" s="171"/>
+      <c r="E66" s="139"/>
       <c r="F66" s="49"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="146"/>
-      <c r="B67" s="148"/>
-      <c r="C67" s="146"/>
-      <c r="D67" s="147"/>
-      <c r="E67" s="148"/>
+      <c r="A67" s="138"/>
+      <c r="B67" s="139"/>
+      <c r="C67" s="138"/>
+      <c r="D67" s="171"/>
+      <c r="E67" s="139"/>
       <c r="F67" s="49"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="146"/>
-      <c r="B68" s="148"/>
-      <c r="C68" s="146"/>
-      <c r="D68" s="147"/>
-      <c r="E68" s="148"/>
+      <c r="A68" s="138"/>
+      <c r="B68" s="139"/>
+      <c r="C68" s="138"/>
+      <c r="D68" s="171"/>
+      <c r="E68" s="139"/>
       <c r="F68" s="49"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="146"/>
-      <c r="B69" s="148"/>
-      <c r="C69" s="146"/>
-      <c r="D69" s="147"/>
-      <c r="E69" s="148"/>
+      <c r="A69" s="138"/>
+      <c r="B69" s="139"/>
+      <c r="C69" s="138"/>
+      <c r="D69" s="171"/>
+      <c r="E69" s="139"/>
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="149"/>
-      <c r="B70" s="151"/>
-      <c r="C70" s="149"/>
-      <c r="D70" s="150"/>
-      <c r="E70" s="151"/>
+      <c r="A70" s="165"/>
+      <c r="B70" s="166"/>
+      <c r="C70" s="165"/>
+      <c r="D70" s="172"/>
+      <c r="E70" s="166"/>
       <c r="F70" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="A69:B69"/>
@@ -5149,52 +5129,39 @@
     <mergeCell ref="C52:E52"/>
     <mergeCell ref="C53:E53"/>
     <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -5435,10 +5402,10 @@
         <v>91</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="139" t="s">
+      <c r="C14" s="180" t="s">
         <v>179</v>
       </c>
-      <c r="D14" s="139"/>
+      <c r="D14" s="180"/>
       <c r="E14" s="54"/>
       <c r="F14" s="54"/>
       <c r="G14" s="54"/>
@@ -5452,10 +5419,10 @@
         <v>136</v>
       </c>
       <c r="B15" s="121"/>
-      <c r="C15" s="140" t="s">
+      <c r="C15" s="164" t="s">
         <v>177</v>
       </c>
-      <c r="D15" s="140"/>
+      <c r="D15" s="164"/>
       <c r="E15" s="95" t="s">
         <v>137</v>
       </c>
@@ -5470,8 +5437,8 @@
         <v>138</v>
       </c>
       <c r="B16" s="121"/>
-      <c r="C16" s="141"/>
-      <c r="D16" s="140"/>
+      <c r="C16" s="163"/>
+      <c r="D16" s="164"/>
       <c r="E16" s="55" t="s">
         <v>175</v>
       </c>
@@ -5521,15 +5488,15 @@
       <c r="L18"/>
     </row>
     <row r="19" spans="1:22">
-      <c r="A19" s="178" t="s">
+      <c r="A19" s="156" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="178"/>
-      <c r="C19" s="178"/>
-      <c r="D19" s="178"/>
-      <c r="E19" s="178"/>
-      <c r="F19" s="178"/>
-      <c r="G19" s="178"/>
+      <c r="B19" s="156"/>
+      <c r="C19" s="156"/>
+      <c r="D19" s="156"/>
+      <c r="E19" s="156"/>
+      <c r="F19" s="156"/>
+      <c r="G19" s="156"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -5539,14 +5506,14 @@
       <c r="A20" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="172" t="s">
+      <c r="B20" s="150" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="173"/>
-      <c r="D20" s="173"/>
-      <c r="E20" s="173"/>
-      <c r="F20" s="173"/>
-      <c r="G20" s="174"/>
+      <c r="C20" s="151"/>
+      <c r="D20" s="151"/>
+      <c r="E20" s="151"/>
+      <c r="F20" s="151"/>
+      <c r="G20" s="152"/>
       <c r="H20" s="105"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -5564,12 +5531,12 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="116"/>
-      <c r="B21" s="161"/>
-      <c r="C21" s="161"/>
-      <c r="D21" s="161"/>
-      <c r="E21" s="161"/>
-      <c r="F21" s="161"/>
-      <c r="G21" s="161"/>
+      <c r="B21" s="167"/>
+      <c r="C21" s="167"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="167"/>
+      <c r="F21" s="167"/>
+      <c r="G21" s="167"/>
       <c r="H21" s="112"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -5587,12 +5554,12 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="117"/>
-      <c r="B22" s="157"/>
-      <c r="C22" s="157"/>
-      <c r="D22" s="157"/>
-      <c r="E22" s="157"/>
-      <c r="F22" s="157"/>
-      <c r="G22" s="157"/>
+      <c r="B22" s="168"/>
+      <c r="C22" s="168"/>
+      <c r="D22" s="168"/>
+      <c r="E22" s="168"/>
+      <c r="F22" s="168"/>
+      <c r="G22" s="168"/>
       <c r="H22" s="112"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -5610,12 +5577,12 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="118"/>
-      <c r="B23" s="159"/>
-      <c r="C23" s="159"/>
-      <c r="D23" s="159"/>
-      <c r="E23" s="159"/>
-      <c r="F23" s="159"/>
-      <c r="G23" s="159"/>
+      <c r="B23" s="169"/>
+      <c r="C23" s="169"/>
+      <c r="D23" s="169"/>
+      <c r="E23" s="169"/>
+      <c r="F23" s="169"/>
+      <c r="G23" s="169"/>
       <c r="H23" s="112"/>
       <c r="M23" s="112"/>
       <c r="N23" s="112"/>
@@ -5635,15 +5602,15 @@
       <c r="L24" s="105"/>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="175" t="s">
+      <c r="A25" s="153" t="s">
         <v>152</v>
       </c>
-      <c r="B25" s="176"/>
-      <c r="C25" s="176"/>
-      <c r="D25" s="176"/>
-      <c r="E25" s="176"/>
-      <c r="F25" s="176"/>
-      <c r="G25" s="177"/>
+      <c r="B25" s="154"/>
+      <c r="C25" s="154"/>
+      <c r="D25" s="154"/>
+      <c r="E25" s="154"/>
+      <c r="F25" s="154"/>
+      <c r="G25" s="155"/>
       <c r="I25" s="105"/>
       <c r="J25" s="105"/>
       <c r="K25" s="105"/>
@@ -5653,14 +5620,14 @@
       <c r="A26" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="152" t="s">
+      <c r="B26" s="173" t="s">
         <v>144</v>
       </c>
-      <c r="C26" s="152"/>
-      <c r="D26" s="152"/>
-      <c r="E26" s="152"/>
-      <c r="F26" s="152"/>
-      <c r="G26" s="152"/>
+      <c r="C26" s="173"/>
+      <c r="D26" s="173"/>
+      <c r="E26" s="173"/>
+      <c r="F26" s="173"/>
+      <c r="G26" s="173"/>
       <c r="H26" s="105"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -5678,12 +5645,12 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="116"/>
-      <c r="B27" s="153"/>
-      <c r="C27" s="153"/>
-      <c r="D27" s="153"/>
-      <c r="E27" s="153"/>
-      <c r="F27" s="153"/>
-      <c r="G27" s="153"/>
+      <c r="B27" s="174"/>
+      <c r="C27" s="174"/>
+      <c r="D27" s="174"/>
+      <c r="E27" s="174"/>
+      <c r="F27" s="174"/>
+      <c r="G27" s="174"/>
       <c r="H27" s="112"/>
       <c r="I27"/>
       <c r="J27"/>
@@ -5701,12 +5668,12 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="117"/>
-      <c r="B28" s="154"/>
-      <c r="C28" s="154"/>
-      <c r="D28" s="154"/>
-      <c r="E28" s="154"/>
-      <c r="F28" s="154"/>
-      <c r="G28" s="154"/>
+      <c r="B28" s="175"/>
+      <c r="C28" s="175"/>
+      <c r="D28" s="175"/>
+      <c r="E28" s="175"/>
+      <c r="F28" s="175"/>
+      <c r="G28" s="175"/>
       <c r="H28" s="112"/>
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
@@ -5720,12 +5687,12 @@
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="118"/>
-      <c r="B29" s="155"/>
-      <c r="C29" s="155"/>
-      <c r="D29" s="155"/>
-      <c r="E29" s="155"/>
-      <c r="F29" s="155"/>
-      <c r="G29" s="155"/>
+      <c r="B29" s="176"/>
+      <c r="C29" s="176"/>
+      <c r="D29" s="176"/>
+      <c r="E29" s="176"/>
+      <c r="F29" s="176"/>
+      <c r="G29" s="176"/>
       <c r="H29" s="112"/>
       <c r="I29" s="105"/>
       <c r="J29" s="105"/>
@@ -5764,15 +5731,15 @@
       <c r="T30"/>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="175" t="s">
+      <c r="A31" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="B31" s="176"/>
-      <c r="C31" s="176"/>
-      <c r="D31" s="176"/>
-      <c r="E31" s="176"/>
-      <c r="F31" s="176"/>
-      <c r="G31" s="177"/>
+      <c r="B31" s="154"/>
+      <c r="C31" s="154"/>
+      <c r="D31" s="154"/>
+      <c r="E31" s="154"/>
+      <c r="F31" s="154"/>
+      <c r="G31" s="155"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
       <c r="K31" s="112"/>
@@ -5782,14 +5749,14 @@
       <c r="A32" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="152" t="s">
+      <c r="B32" s="173" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="152"/>
-      <c r="D32" s="152"/>
-      <c r="E32" s="152"/>
-      <c r="F32" s="152"/>
-      <c r="G32" s="152"/>
+      <c r="C32" s="173"/>
+      <c r="D32" s="173"/>
+      <c r="E32" s="173"/>
+      <c r="F32" s="173"/>
+      <c r="G32" s="173"/>
       <c r="H32" s="105"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -5807,12 +5774,12 @@
     </row>
     <row r="33" spans="1:26">
       <c r="A33" s="116"/>
-      <c r="B33" s="161"/>
-      <c r="C33" s="161"/>
-      <c r="D33" s="161"/>
-      <c r="E33" s="161"/>
-      <c r="F33" s="161"/>
-      <c r="G33" s="197"/>
+      <c r="B33" s="167"/>
+      <c r="C33" s="167"/>
+      <c r="D33" s="167"/>
+      <c r="E33" s="167"/>
+      <c r="F33" s="167"/>
+      <c r="G33" s="187"/>
       <c r="H33" s="112"/>
       <c r="I33"/>
       <c r="J33"/>
@@ -5830,12 +5797,12 @@
     </row>
     <row r="34" spans="1:26">
       <c r="A34" s="117"/>
-      <c r="B34" s="157"/>
-      <c r="C34" s="157"/>
-      <c r="D34" s="157"/>
-      <c r="E34" s="157"/>
-      <c r="F34" s="157"/>
-      <c r="G34" s="158"/>
+      <c r="B34" s="168"/>
+      <c r="C34" s="168"/>
+      <c r="D34" s="168"/>
+      <c r="E34" s="168"/>
+      <c r="F34" s="168"/>
+      <c r="G34" s="178"/>
       <c r="H34" s="112"/>
       <c r="M34" s="112"/>
       <c r="N34" s="112"/>
@@ -5849,12 +5816,12 @@
     </row>
     <row r="35" spans="1:26">
       <c r="A35" s="118"/>
-      <c r="B35" s="159"/>
-      <c r="C35" s="159"/>
-      <c r="D35" s="159"/>
-      <c r="E35" s="159"/>
-      <c r="F35" s="159"/>
-      <c r="G35" s="160"/>
+      <c r="B35" s="169"/>
+      <c r="C35" s="169"/>
+      <c r="D35" s="169"/>
+      <c r="E35" s="169"/>
+      <c r="F35" s="169"/>
+      <c r="G35" s="179"/>
       <c r="H35" s="112"/>
       <c r="M35" s="112"/>
       <c r="N35" s="112"/>
@@ -5918,82 +5885,82 @@
       <c r="Z38" s="39"/>
     </row>
     <row r="39" spans="1:26">
-      <c r="A39" s="185" t="s">
+      <c r="A39" s="189" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="185" t="s">
+      <c r="B39" s="189" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="187" t="s">
+      <c r="C39" s="191" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="185" t="s">
+      <c r="D39" s="189" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="188" t="s">
+      <c r="E39" s="192" t="s">
         <v>132</v>
       </c>
-      <c r="F39" s="188" t="s">
+      <c r="F39" s="192" t="s">
         <v>138</v>
       </c>
-      <c r="G39" s="185" t="s">
+      <c r="G39" s="189" t="s">
         <v>13</v>
       </c>
-      <c r="H39" s="185" t="s">
+      <c r="H39" s="189" t="s">
         <v>95</v>
       </c>
-      <c r="I39" s="192" t="s">
+      <c r="I39" s="188" t="s">
         <v>158</v>
       </c>
-      <c r="J39" s="192" t="s">
+      <c r="J39" s="188" t="s">
         <v>159</v>
       </c>
-      <c r="K39" s="192" t="s">
+      <c r="K39" s="188" t="s">
         <v>160</v>
       </c>
-      <c r="L39" s="193" t="s">
+      <c r="L39" s="196" t="s">
         <v>161</v>
       </c>
-      <c r="M39" s="185" t="s">
+      <c r="M39" s="189" t="s">
         <v>154</v>
       </c>
-      <c r="N39" s="185" t="s">
+      <c r="N39" s="189" t="s">
         <v>164</v>
       </c>
-      <c r="O39" s="187" t="s">
+      <c r="O39" s="191" t="s">
         <v>163</v>
       </c>
-      <c r="P39" s="195" t="s">
+      <c r="P39" s="185" t="s">
         <v>71</v>
       </c>
-      <c r="Q39" s="196"/>
-      <c r="R39" s="195" t="s">
+      <c r="Q39" s="186"/>
+      <c r="R39" s="185" t="s">
         <v>17</v>
       </c>
-      <c r="S39" s="196"/>
+      <c r="S39" s="186"/>
       <c r="T39" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="U39" s="185" t="s">
+      <c r="U39" s="189" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:26">
-      <c r="A40" s="186"/>
-      <c r="B40" s="186"/>
-      <c r="C40" s="186"/>
-      <c r="D40" s="186"/>
-      <c r="E40" s="189"/>
-      <c r="F40" s="190"/>
-      <c r="G40" s="186"/>
-      <c r="H40" s="186"/>
-      <c r="I40" s="192"/>
-      <c r="J40" s="192"/>
-      <c r="K40" s="192"/>
-      <c r="L40" s="194"/>
-      <c r="M40" s="191"/>
-      <c r="N40" s="191"/>
-      <c r="O40" s="191"/>
+      <c r="A40" s="190"/>
+      <c r="B40" s="190"/>
+      <c r="C40" s="190"/>
+      <c r="D40" s="190"/>
+      <c r="E40" s="193"/>
+      <c r="F40" s="194"/>
+      <c r="G40" s="190"/>
+      <c r="H40" s="190"/>
+      <c r="I40" s="188"/>
+      <c r="J40" s="188"/>
+      <c r="K40" s="188"/>
+      <c r="L40" s="197"/>
+      <c r="M40" s="195"/>
+      <c r="N40" s="195"/>
+      <c r="O40" s="195"/>
       <c r="P40" s="29" t="s">
         <v>75</v>
       </c>
@@ -6009,7 +5976,7 @@
       <c r="T40" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="U40" s="186"/>
+      <c r="U40" s="190"/>
     </row>
     <row r="41" spans="1:26" ht="45">
       <c r="A41" s="7">
@@ -6600,26 +6567,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="R39:S39"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="P39:Q39"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="U39:U40"/>
     <mergeCell ref="A39:A40"/>
@@ -6636,6 +6583,26 @@
     <mergeCell ref="L39:L40"/>
     <mergeCell ref="N39:N40"/>
     <mergeCell ref="M39:M40"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="R39:S39"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="K39:K40"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -6868,10 +6835,10 @@
         <v>136</v>
       </c>
       <c r="B12" s="121"/>
-      <c r="C12" s="140" t="s">
+      <c r="C12" s="164" t="s">
         <v>177</v>
       </c>
-      <c r="D12" s="140"/>
+      <c r="D12" s="164"/>
       <c r="E12" s="95" t="s">
         <v>137</v>
       </c>
@@ -6886,8 +6853,8 @@
         <v>138</v>
       </c>
       <c r="B13" s="121"/>
-      <c r="C13" s="140"/>
-      <c r="D13" s="140"/>
+      <c r="C13" s="164"/>
+      <c r="D13" s="164"/>
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="54"/>
@@ -6927,15 +6894,15 @@
       <c r="L15"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="178" t="s">
+      <c r="A16" s="156" t="s">
         <v>151</v>
       </c>
-      <c r="B16" s="178"/>
-      <c r="C16" s="178"/>
-      <c r="D16" s="178"/>
-      <c r="E16" s="178"/>
-      <c r="F16" s="178"/>
-      <c r="G16" s="178"/>
+      <c r="B16" s="156"/>
+      <c r="C16" s="156"/>
+      <c r="D16" s="156"/>
+      <c r="E16" s="156"/>
+      <c r="F16" s="156"/>
+      <c r="G16" s="156"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -6946,14 +6913,14 @@
       <c r="A17" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="172" t="s">
+      <c r="B17" s="150" t="s">
         <v>143</v>
       </c>
-      <c r="C17" s="173"/>
-      <c r="D17" s="173"/>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="174"/>
+      <c r="C17" s="151"/>
+      <c r="D17" s="151"/>
+      <c r="E17" s="151"/>
+      <c r="F17" s="151"/>
+      <c r="G17" s="152"/>
       <c r="H17" s="105"/>
       <c r="I17"/>
       <c r="J17"/>
@@ -6969,12 +6936,12 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="116"/>
-      <c r="B18" s="161"/>
-      <c r="C18" s="161"/>
-      <c r="D18" s="161"/>
-      <c r="E18" s="161"/>
-      <c r="F18" s="161"/>
-      <c r="G18" s="161"/>
+      <c r="B18" s="167"/>
+      <c r="C18" s="167"/>
+      <c r="D18" s="167"/>
+      <c r="E18" s="167"/>
+      <c r="F18" s="167"/>
+      <c r="G18" s="167"/>
       <c r="H18" s="112"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -6989,12 +6956,12 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="117"/>
-      <c r="B19" s="157"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="157"/>
+      <c r="B19" s="168"/>
+      <c r="C19" s="168"/>
+      <c r="D19" s="168"/>
+      <c r="E19" s="168"/>
+      <c r="F19" s="168"/>
+      <c r="G19" s="168"/>
       <c r="H19" s="112"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -7009,12 +6976,12 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="118"/>
-      <c r="B20" s="159"/>
-      <c r="C20" s="159"/>
-      <c r="D20" s="159"/>
-      <c r="E20" s="159"/>
-      <c r="F20" s="159"/>
-      <c r="G20" s="159"/>
+      <c r="B20" s="169"/>
+      <c r="C20" s="169"/>
+      <c r="D20" s="169"/>
+      <c r="E20" s="169"/>
+      <c r="F20" s="169"/>
+      <c r="G20" s="169"/>
       <c r="H20" s="112"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -7041,15 +7008,15 @@
       <c r="O21" s="112"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="175" t="s">
+      <c r="A22" s="153" t="s">
         <v>152</v>
       </c>
-      <c r="B22" s="176"/>
-      <c r="C22" s="176"/>
-      <c r="D22" s="176"/>
-      <c r="E22" s="176"/>
-      <c r="F22" s="176"/>
-      <c r="G22" s="177"/>
+      <c r="B22" s="154"/>
+      <c r="C22" s="154"/>
+      <c r="D22" s="154"/>
+      <c r="E22" s="154"/>
+      <c r="F22" s="154"/>
+      <c r="G22" s="155"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -7062,14 +7029,14 @@
       <c r="A23" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="152" t="s">
+      <c r="B23" s="173" t="s">
         <v>144</v>
       </c>
-      <c r="C23" s="152"/>
-      <c r="D23" s="152"/>
-      <c r="E23" s="152"/>
-      <c r="F23" s="152"/>
-      <c r="G23" s="152"/>
+      <c r="C23" s="173"/>
+      <c r="D23" s="173"/>
+      <c r="E23" s="173"/>
+      <c r="F23" s="173"/>
+      <c r="G23" s="173"/>
       <c r="H23" s="105"/>
       <c r="M23" s="112"/>
       <c r="N23" s="112"/>
@@ -7083,12 +7050,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="116"/>
-      <c r="B24" s="153"/>
-      <c r="C24" s="153"/>
-      <c r="D24" s="153"/>
-      <c r="E24" s="153"/>
-      <c r="F24" s="153"/>
-      <c r="G24" s="153"/>
+      <c r="B24" s="174"/>
+      <c r="C24" s="174"/>
+      <c r="D24" s="174"/>
+      <c r="E24" s="174"/>
+      <c r="F24" s="174"/>
+      <c r="G24" s="174"/>
       <c r="H24" s="112"/>
       <c r="I24" s="105"/>
       <c r="J24" s="105"/>
@@ -7103,12 +7070,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="117"/>
-      <c r="B25" s="154"/>
-      <c r="C25" s="154"/>
-      <c r="D25" s="154"/>
-      <c r="E25" s="154"/>
-      <c r="F25" s="154"/>
-      <c r="G25" s="154"/>
+      <c r="B25" s="175"/>
+      <c r="C25" s="175"/>
+      <c r="D25" s="175"/>
+      <c r="E25" s="175"/>
+      <c r="F25" s="175"/>
+      <c r="G25" s="175"/>
       <c r="H25" s="112"/>
       <c r="I25" s="105"/>
       <c r="J25" s="105"/>
@@ -7123,12 +7090,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="118"/>
-      <c r="B26" s="155"/>
-      <c r="C26" s="155"/>
-      <c r="D26" s="155"/>
-      <c r="E26" s="155"/>
-      <c r="F26" s="155"/>
-      <c r="G26" s="155"/>
+      <c r="B26" s="176"/>
+      <c r="C26" s="176"/>
+      <c r="D26" s="176"/>
+      <c r="E26" s="176"/>
+      <c r="F26" s="176"/>
+      <c r="G26" s="176"/>
       <c r="H26" s="112"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -7167,15 +7134,15 @@
       <c r="T27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="175" t="s">
+      <c r="A28" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="B28" s="176"/>
-      <c r="C28" s="176"/>
-      <c r="D28" s="176"/>
-      <c r="E28" s="176"/>
-      <c r="F28" s="176"/>
-      <c r="G28" s="177"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="154"/>
+      <c r="D28" s="154"/>
+      <c r="E28" s="154"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="155"/>
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
       <c r="O28" s="112"/>
@@ -7184,14 +7151,14 @@
       <c r="A29" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="152" t="s">
+      <c r="B29" s="173" t="s">
         <v>145</v>
       </c>
-      <c r="C29" s="152"/>
-      <c r="D29" s="152"/>
-      <c r="E29" s="152"/>
-      <c r="F29" s="152"/>
-      <c r="G29" s="152"/>
+      <c r="C29" s="173"/>
+      <c r="D29" s="173"/>
+      <c r="E29" s="173"/>
+      <c r="F29" s="173"/>
+      <c r="G29" s="173"/>
       <c r="H29" s="105"/>
       <c r="I29" s="105"/>
       <c r="J29" s="105"/>
@@ -7209,12 +7176,12 @@
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="116"/>
-      <c r="B30" s="161"/>
-      <c r="C30" s="161"/>
-      <c r="D30" s="161"/>
-      <c r="E30" s="161"/>
-      <c r="F30" s="161"/>
-      <c r="G30" s="197"/>
+      <c r="B30" s="167"/>
+      <c r="C30" s="167"/>
+      <c r="D30" s="167"/>
+      <c r="E30" s="167"/>
+      <c r="F30" s="167"/>
+      <c r="G30" s="187"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -7232,12 +7199,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="117"/>
-      <c r="B31" s="157"/>
-      <c r="C31" s="157"/>
-      <c r="D31" s="157"/>
-      <c r="E31" s="157"/>
-      <c r="F31" s="157"/>
-      <c r="G31" s="158"/>
+      <c r="B31" s="168"/>
+      <c r="C31" s="168"/>
+      <c r="D31" s="168"/>
+      <c r="E31" s="168"/>
+      <c r="F31" s="168"/>
+      <c r="G31" s="178"/>
       <c r="H31" s="112"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
@@ -7252,12 +7219,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="118"/>
-      <c r="B32" s="159"/>
-      <c r="C32" s="159"/>
-      <c r="D32" s="159"/>
-      <c r="E32" s="159"/>
-      <c r="F32" s="159"/>
-      <c r="G32" s="160"/>
+      <c r="B32" s="169"/>
+      <c r="C32" s="169"/>
+      <c r="D32" s="169"/>
+      <c r="E32" s="169"/>
+      <c r="F32" s="169"/>
+      <c r="G32" s="179"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -7327,84 +7294,84 @@
       <c r="U35" s="58"/>
     </row>
     <row r="36" spans="1:21" ht="30" customHeight="1">
-      <c r="A36" s="188" t="s">
+      <c r="A36" s="192" t="s">
         <v>97</v>
       </c>
-      <c r="B36" s="188" t="s">
+      <c r="B36" s="192" t="s">
         <v>98</v>
       </c>
       <c r="C36" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="188" t="s">
+      <c r="D36" s="192" t="s">
         <v>92</v>
       </c>
-      <c r="E36" s="188" t="s">
+      <c r="E36" s="192" t="s">
         <v>132</v>
       </c>
-      <c r="F36" s="188" t="s">
+      <c r="F36" s="192" t="s">
         <v>138</v>
       </c>
-      <c r="G36" s="188" t="s">
+      <c r="G36" s="192" t="s">
         <v>111</v>
       </c>
-      <c r="H36" s="188" t="s">
+      <c r="H36" s="192" t="s">
         <v>110</v>
       </c>
-      <c r="I36" s="203" t="s">
+      <c r="I36" s="202" t="s">
         <v>158</v>
       </c>
-      <c r="J36" s="205" t="s">
+      <c r="J36" s="204" t="s">
         <v>159</v>
       </c>
-      <c r="K36" s="205" t="s">
+      <c r="K36" s="204" t="s">
         <v>160</v>
       </c>
-      <c r="L36" s="193" t="s">
+      <c r="L36" s="196" t="s">
         <v>161</v>
       </c>
-      <c r="M36" s="185" t="s">
+      <c r="M36" s="189" t="s">
         <v>154</v>
       </c>
-      <c r="N36" s="185" t="s">
+      <c r="N36" s="189" t="s">
         <v>164</v>
       </c>
-      <c r="O36" s="187" t="s">
+      <c r="O36" s="191" t="s">
         <v>163</v>
       </c>
-      <c r="P36" s="202" t="s">
+      <c r="P36" s="201" t="s">
         <v>101</v>
       </c>
-      <c r="Q36" s="200"/>
-      <c r="R36" s="199" t="s">
+      <c r="Q36" s="199"/>
+      <c r="R36" s="198" t="s">
         <v>102</v>
       </c>
-      <c r="S36" s="200"/>
+      <c r="S36" s="199"/>
       <c r="T36" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="U36" s="188" t="s">
+      <c r="U36" s="192" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15">
-      <c r="A37" s="201"/>
-      <c r="B37" s="201"/>
+      <c r="A37" s="200"/>
+      <c r="B37" s="200"/>
       <c r="C37" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="D37" s="201"/>
-      <c r="E37" s="190"/>
-      <c r="F37" s="190"/>
-      <c r="G37" s="201"/>
-      <c r="H37" s="201"/>
-      <c r="I37" s="204"/>
-      <c r="J37" s="206"/>
-      <c r="K37" s="206"/>
-      <c r="L37" s="194"/>
-      <c r="M37" s="191"/>
-      <c r="N37" s="191"/>
-      <c r="O37" s="198"/>
+      <c r="D37" s="200"/>
+      <c r="E37" s="194"/>
+      <c r="F37" s="194"/>
+      <c r="G37" s="200"/>
+      <c r="H37" s="200"/>
+      <c r="I37" s="203"/>
+      <c r="J37" s="205"/>
+      <c r="K37" s="205"/>
+      <c r="L37" s="197"/>
+      <c r="M37" s="195"/>
+      <c r="N37" s="195"/>
+      <c r="O37" s="206"/>
       <c r="P37" s="62" t="s">
         <v>105</v>
       </c>
@@ -7420,7 +7387,7 @@
       <c r="T37" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="U37" s="201"/>
+      <c r="U37" s="200"/>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="64">
@@ -8020,6 +7987,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="O36:O37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="M36:M37"/>
     <mergeCell ref="R36:S36"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="B29:G29"/>
@@ -8036,24 +8021,6 @@
     <mergeCell ref="I36:I37"/>
     <mergeCell ref="J36:J37"/>
     <mergeCell ref="K36:K37"/>
-    <mergeCell ref="O36:O37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">

</xml_diff>